<commit_message>
Implement more fix/change requests
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2578" uniqueCount="1496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="1500">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -3523,6 +3523,18 @@
   </si>
   <si>
     <t xml:space="preserve">15a. Ikiwa mwaka haujulikani tafadhali jaza umri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q15b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16b. Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16b. Género</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16b. Jinsia</t>
   </si>
   <si>
     <t xml:space="preserve">q16</t>
@@ -4868,7 +4880,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.17578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -5919,7 +5931,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.17578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.67"/>
@@ -7403,12 +7415,12 @@
   <dimension ref="A1:Y1011"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B213" activeCellId="0" sqref="B213"/>
+      <selection pane="bottomLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.17578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -11198,7 +11210,7 @@
       <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.17578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -29626,7 +29638,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.17578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.04"/>
@@ -30760,12 +30772,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D356"/>
+  <dimension ref="A1:D357"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D315" activeCellId="0" sqref="D315"/>
+      <selection pane="bottomLeft" activeCell="D270" activeCellId="0" sqref="D270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34444,38 +34456,38 @@
         <v>1170</v>
       </c>
       <c r="B270" s="13" t="s">
-        <v>1119</v>
+        <v>1171</v>
       </c>
       <c r="C270" s="13" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="D270" s="13" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="13" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="B271" s="13" t="s">
-        <v>1174</v>
+        <v>1119</v>
       </c>
       <c r="C271" s="13" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="D271" s="13" t="s">
-        <v>1174</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="13" t="s">
-        <v>1175</v>
+        <v>1177</v>
       </c>
       <c r="B272" s="13" t="s">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="C272" s="13" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D272" s="13" t="s">
         <v>1178</v>
@@ -34556,27 +34568,27 @@
         <v>1199</v>
       </c>
       <c r="B278" s="13" t="s">
-        <v>1119</v>
+        <v>1200</v>
       </c>
       <c r="C278" s="13" t="s">
-        <v>1171</v>
+        <v>1201</v>
       </c>
       <c r="D278" s="13" t="s">
-        <v>1172</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="13" t="s">
-        <v>1200</v>
+        <v>1203</v>
       </c>
       <c r="B279" s="13" t="s">
-        <v>1201</v>
+        <v>1119</v>
       </c>
       <c r="C279" s="13" t="s">
-        <v>1202</v>
+        <v>1175</v>
       </c>
       <c r="D279" s="13" t="s">
-        <v>1203</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34747,17 +34759,17 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="13" t="s">
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="13" t="s">
         <v>1252</v>
       </c>
-      <c r="B293" s="13" t="s">
+      <c r="B292" s="13" t="s">
         <v>1253</v>
       </c>
-      <c r="C293" s="13" t="s">
+      <c r="C292" s="13" t="s">
         <v>1254</v>
       </c>
-      <c r="D293" s="13" t="s">
+      <c r="D292" s="13" t="s">
         <v>1255</v>
       </c>
     </row>
@@ -35090,18 +35102,18 @@
       <c r="B317" s="13" t="s">
         <v>1349</v>
       </c>
+      <c r="C317" s="13" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D317" s="13" t="s">
+        <v>1351</v>
+      </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="13" t="s">
-        <v>1350</v>
+        <v>1352</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>1351</v>
-      </c>
-      <c r="C318" s="13" t="s">
-        <v>1352</v>
-      </c>
-      <c r="D318" s="13" t="s">
         <v>1353</v>
       </c>
     </row>
@@ -35413,17 +35425,17 @@
         <v>1441</v>
       </c>
     </row>
-    <row r="342" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="13" t="s">
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="13" t="s">
         <v>1442</v>
       </c>
-      <c r="B342" s="13" t="s">
+      <c r="B341" s="13" t="s">
         <v>1443</v>
       </c>
-      <c r="C342" s="14" t="s">
+      <c r="C341" s="13" t="s">
         <v>1444</v>
       </c>
-      <c r="D342" s="14" t="s">
+      <c r="D341" s="13" t="s">
         <v>1445</v>
       </c>
     </row>
@@ -35455,7 +35467,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="345" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="13" t="s">
         <v>1454</v>
       </c>
@@ -35483,7 +35495,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="13" t="s">
         <v>1462</v>
       </c>
@@ -35525,7 +35537,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="350" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="13" t="s">
         <v>1474</v>
       </c>
@@ -35539,11 +35551,11 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="16.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="351" customFormat="false" ht="34.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="13" t="s">
         <v>1478</v>
       </c>
-      <c r="B351" s="16" t="s">
+      <c r="B351" s="13" t="s">
         <v>1479</v>
       </c>
       <c r="C351" s="14" t="s">
@@ -35553,17 +35565,17 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" customFormat="false" ht="16.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="13" t="s">
         <v>1482</v>
       </c>
-      <c r="B352" s="13" t="s">
+      <c r="B352" s="16" t="s">
         <v>1483</v>
       </c>
-      <c r="C352" s="13" t="s">
+      <c r="C352" s="14" t="s">
         <v>1484</v>
       </c>
-      <c r="D352" s="13" t="s">
+      <c r="D352" s="14" t="s">
         <v>1485</v>
       </c>
     </row>
@@ -35581,50 +35593,64 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="354" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="13" t="s">
         <v>1490</v>
       </c>
       <c r="B354" s="13" t="s">
         <v>1491</v>
       </c>
-      <c r="C354" s="14" t="s">
-        <v>1087</v>
-      </c>
-      <c r="D354" s="14" t="s">
-        <v>1088</v>
+      <c r="C354" s="13" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D354" s="13" t="s">
+        <v>1493</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="13" t="s">
-        <v>1492</v>
+        <v>1494</v>
       </c>
       <c r="B355" s="13" t="s">
-        <v>1493</v>
+        <v>1495</v>
       </c>
       <c r="C355" s="14" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
       <c r="D355" s="14" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="13" t="s">
-        <v>1494</v>
+        <v>1496</v>
       </c>
       <c r="B356" s="13" t="s">
-        <v>1495</v>
+        <v>1497</v>
       </c>
       <c r="C356" s="14" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D356" s="14" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="22.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="13" t="s">
+        <v>1498</v>
+      </c>
+      <c r="B357" s="13" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C357" s="14" t="s">
         <v>1095</v>
       </c>
-      <c r="D356" s="14" t="s">
+      <c r="D357" s="14" t="s">
         <v>1096</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:D1 B251:D259 B263:D263 B266:D291 B352:B1048576 C69:D212 C225:D225 C249:D341 D357:D1048576 C352:D353 C227:D230 C355:C1048576 B1:B350 C219:D222 C239:D239 C1:D64 C246:C247">
+  <conditionalFormatting sqref="B1:D1 B251:D259 B263:D263 B266:D292 B353:B1048576 C69:D212 C225:D225 C249:D342 D358:D1048576 C353:D354 C227:D230 C356:C1048576 B1:B351 C219:D222 C239:D239 C1:D64 C246:C247">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Implement form change requests
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3465" uniqueCount="1792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3469" uniqueCount="1796">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -4126,6 +4126,18 @@
   </si>
   <si>
     <t xml:space="preserve">Ingiza mwaka kati ya 1920 na 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year_hint_new_born</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter a year between 2020 and 2021. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insira um ano entre 2020 e 2021.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingiza mwaka kati ya 2020 na 2021</t>
   </si>
   <si>
     <t xml:space="preserve">date_cons</t>
@@ -5772,7 +5784,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.25390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.2734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -6823,7 +6835,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.67"/>
@@ -8312,7 +8324,7 @@
       <selection pane="bottomLeft" activeCell="A256" activeCellId="0" sqref="A256"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -13552,7 +13564,7 @@
       <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -31977,10 +31989,10 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.25390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.2734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.04"/>
@@ -32040,7 +32052,7 @@
         <v>563</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>20210221001</v>
+        <v>20210222001</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -33121,12 +33133,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D505"/>
+  <dimension ref="A1:D506"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B396" activeCellId="0" sqref="B396"/>
+      <selection pane="bottomLeft" activeCell="D391" activeCellId="0" sqref="D391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38508,17 +38520,17 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="390" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="13" t="s">
         <v>1367</v>
       </c>
       <c r="B390" s="13" t="s">
         <v>1368</v>
       </c>
-      <c r="C390" s="15" t="s">
+      <c r="C390" s="13" t="s">
         <v>1369</v>
       </c>
-      <c r="D390" s="15" t="s">
+      <c r="D390" s="13" t="s">
         <v>1370</v>
       </c>
     </row>
@@ -38550,17 +38562,17 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="393" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="13" t="s">
         <v>1379</v>
       </c>
       <c r="B393" s="13" t="s">
         <v>1380</v>
       </c>
-      <c r="C393" s="13" t="s">
+      <c r="C393" s="15" t="s">
         <v>1381</v>
       </c>
-      <c r="D393" s="13" t="s">
+      <c r="D393" s="15" t="s">
         <v>1382</v>
       </c>
     </row>
@@ -38571,116 +38583,116 @@
       <c r="B394" s="13" t="s">
         <v>1384</v>
       </c>
+      <c r="C394" s="13" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D394" s="13" t="s">
+        <v>1386</v>
+      </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="13" t="s">
-        <v>1385</v>
+        <v>1387</v>
       </c>
       <c r="B395" s="13" t="s">
-        <v>1386</v>
-      </c>
-    </row>
-    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B397" s="13" t="s">
-        <v>1387</v>
-      </c>
-      <c r="C397" s="13" t="s">
         <v>1388</v>
       </c>
-      <c r="D397" s="13" t="s">
+    </row>
+    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A396" s="13" t="s">
         <v>1389</v>
+      </c>
+      <c r="B396" s="13" t="s">
+        <v>1390</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="C398" s="13" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D398" s="13" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="C399" s="13" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D399" s="13" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="13" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B400" s="13" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="C400" s="13" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D400" s="13" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B401" s="13" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="C401" s="13" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D401" s="13" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="C402" s="13" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D402" s="13" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="C403" s="13" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D403" s="13" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="13" t="s">
-        <v>1408</v>
+        <v>70</v>
       </c>
       <c r="B404" s="13" t="s">
         <v>1409</v>
@@ -38865,38 +38877,38 @@
         <v>1460</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>1405</v>
+        <v>1461</v>
       </c>
       <c r="C417" s="13" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D417" s="13" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="13" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>1464</v>
+        <v>1409</v>
       </c>
       <c r="C418" s="13" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D418" s="13" t="s">
-        <v>1464</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="13" t="s">
-        <v>1465</v>
+        <v>1467</v>
       </c>
       <c r="B419" s="13" t="s">
-        <v>1466</v>
+        <v>1468</v>
       </c>
       <c r="C419" s="13" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D419" s="13" t="s">
         <v>1468</v>
@@ -38977,27 +38989,27 @@
         <v>1489</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>1405</v>
+        <v>1490</v>
       </c>
       <c r="C425" s="13" t="s">
-        <v>1461</v>
+        <v>1491</v>
       </c>
       <c r="D425" s="13" t="s">
-        <v>1462</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="13" t="s">
-        <v>1490</v>
+        <v>1493</v>
       </c>
       <c r="B426" s="13" t="s">
-        <v>1491</v>
+        <v>1409</v>
       </c>
       <c r="C426" s="13" t="s">
-        <v>1492</v>
+        <v>1465</v>
       </c>
       <c r="D426" s="13" t="s">
-        <v>1493</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39168,17 +39180,17 @@
         <v>1541</v>
       </c>
     </row>
-    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="13" t="s">
+    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A439" s="13" t="s">
         <v>1542</v>
       </c>
-      <c r="B440" s="13" t="s">
+      <c r="B439" s="13" t="s">
         <v>1543</v>
       </c>
-      <c r="C440" s="13" t="s">
+      <c r="C439" s="13" t="s">
         <v>1544</v>
       </c>
-      <c r="D440" s="13" t="s">
+      <c r="D439" s="13" t="s">
         <v>1545</v>
       </c>
     </row>
@@ -39511,18 +39523,18 @@
       <c r="B464" s="13" t="s">
         <v>1639</v>
       </c>
+      <c r="C464" s="13" t="s">
+        <v>1640</v>
+      </c>
+      <c r="D464" s="13" t="s">
+        <v>1641</v>
+      </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="13" t="s">
-        <v>1640</v>
+        <v>1642</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>1641</v>
-      </c>
-      <c r="C465" s="13" t="s">
-        <v>1642</v>
-      </c>
-      <c r="D465" s="13" t="s">
         <v>1643</v>
       </c>
     </row>
@@ -39834,17 +39846,17 @@
         <v>1731</v>
       </c>
     </row>
-    <row r="489" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A489" s="13" t="s">
+    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="13" t="s">
         <v>1732</v>
       </c>
-      <c r="B489" s="13" t="s">
+      <c r="B488" s="13" t="s">
         <v>1733</v>
       </c>
-      <c r="C489" s="15" t="s">
+      <c r="C488" s="13" t="s">
         <v>1734</v>
       </c>
-      <c r="D489" s="15" t="s">
+      <c r="D488" s="13" t="s">
         <v>1735</v>
       </c>
     </row>
@@ -39876,7 +39888,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="492" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="492" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="13" t="s">
         <v>1744</v>
       </c>
@@ -39918,7 +39930,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="495" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="495" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="13" t="s">
         <v>1756</v>
       </c>
@@ -39946,7 +39958,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="497" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="497" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="13" t="s">
         <v>1764</v>
       </c>
@@ -39960,11 +39972,11 @@
         <v>1767</v>
       </c>
     </row>
-    <row r="498" customFormat="false" ht="16.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="498" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="13" t="s">
         <v>1768</v>
       </c>
-      <c r="B498" s="17" t="s">
+      <c r="B498" s="13" t="s">
         <v>1769</v>
       </c>
       <c r="C498" s="15" t="s">
@@ -39974,17 +39986,17 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="499" customFormat="false" ht="16.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A499" s="13" t="s">
         <v>1772</v>
       </c>
-      <c r="B499" s="13" t="s">
+      <c r="B499" s="17" t="s">
         <v>1773</v>
       </c>
-      <c r="C499" s="13" t="s">
+      <c r="C499" s="15" t="s">
         <v>1774</v>
       </c>
-      <c r="D499" s="13" t="s">
+      <c r="D499" s="15" t="s">
         <v>1775</v>
       </c>
     </row>
@@ -40002,26 +40014,26 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="501" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="13" t="s">
         <v>1780</v>
       </c>
       <c r="B501" s="13" t="s">
         <v>1781</v>
       </c>
-      <c r="C501" s="15" t="s">
-        <v>1369</v>
-      </c>
-      <c r="D501" s="15" t="s">
-        <v>1370</v>
+      <c r="C501" s="13" t="s">
+        <v>1782</v>
+      </c>
+      <c r="D501" s="13" t="s">
+        <v>1783</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="13" t="s">
-        <v>1782</v>
+        <v>1784</v>
       </c>
       <c r="B502" s="13" t="s">
-        <v>1783</v>
+        <v>1785</v>
       </c>
       <c r="C502" s="15" t="s">
         <v>1373</v>
@@ -40032,10 +40044,10 @@
     </row>
     <row r="503" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="13" t="s">
-        <v>1784</v>
+        <v>1786</v>
       </c>
       <c r="B503" s="13" t="s">
-        <v>1785</v>
+        <v>1787</v>
       </c>
       <c r="C503" s="15" t="s">
         <v>1377</v>
@@ -40044,36 +40056,50 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A504" s="18" t="s">
-        <v>1786</v>
+    <row r="504" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="13" t="s">
+        <v>1788</v>
       </c>
       <c r="B504" s="13" t="s">
-        <v>1787</v>
-      </c>
-      <c r="C504" s="13" t="s">
-        <v>1787</v>
-      </c>
-      <c r="D504" s="13" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="13" t="s">
-        <v>1788</v>
+        <v>1789</v>
+      </c>
+      <c r="C504" s="15" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D504" s="15" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A505" s="18" t="s">
+        <v>1790</v>
       </c>
       <c r="B505" s="13" t="s">
-        <v>1789</v>
+        <v>1791</v>
       </c>
       <c r="C505" s="13" t="s">
-        <v>1790</v>
+        <v>1791</v>
       </c>
       <c r="D505" s="13" t="s">
         <v>1791</v>
       </c>
     </row>
+    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="13" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B506" s="13" t="s">
+        <v>1793</v>
+      </c>
+      <c r="C506" s="13" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D506" s="13" t="s">
+        <v>1795</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:D1 B397:D405 B409:D409 B412:D438 B505:B1048576 C69:D357 C370:D370 C394:D488 D505:D1048576 C499:D500 C372:D375 C505:C1048576 C364:D367 C384:D384 C1:D64 C391:C392 B499:B503 C502:C503 B504:D504 B1:B497">
+  <conditionalFormatting sqref="B1:D1 B398:D406 B410:D410 B413:D439 B506:B1048576 C69:D357 C370:D370 C395:D489 D506:D1048576 C500:D501 C372:D375 C506:C1048576 C364:D367 C384:D384 C1:D64 C392:C393 B500:B504 C503:C504 B505:D505 B1:B498">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fix emigrated date and departure date
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="1800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="1800">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -489,6 +489,9 @@
     <t xml:space="preserve">dmy_ago_dk</t>
   </si>
   <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
     <t xml:space="preserve">days_ago</t>
   </si>
   <si>
@@ -819,9 +822,6 @@
     <t xml:space="preserve">tomorrow</t>
   </si>
   <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
     <t xml:space="preserve">time_awake</t>
   </si>
   <si>
@@ -3798,13 +3798,13 @@
     <t xml:space="preserve">or_enter_num</t>
   </si>
   <si>
-    <t xml:space="preserve">or enter number </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ou digite um número</t>
-  </si>
-  <si>
-    <t xml:space="preserve">au ingiza namba</t>
+    <t xml:space="preserve">enter number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">digite um número</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingiza namba</t>
   </si>
   <si>
     <t xml:space="preserve">days_weeks_months_years</t>
@@ -8328,12 +8328,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1013"/>
+  <dimension ref="A1:Y1014"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C209" activeCellId="0" sqref="C209"/>
+      <selection pane="bottomLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.33984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9571,26 +9571,26 @@
         <v>153</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>158</v>
+        <v>42</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>158</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>159</v>
@@ -9601,7 +9601,7 @@
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>160</v>
@@ -9612,7 +9612,7 @@
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>161</v>
@@ -9623,18 +9623,18 @@
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B99" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B99" s="0" t="s">
-        <v>163</v>
-      </c>
       <c r="C99" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>164</v>
@@ -9645,7 +9645,7 @@
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B101" s="0" t="s">
         <v>165</v>
@@ -9656,7 +9656,7 @@
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>166</v>
@@ -9667,7 +9667,7 @@
     </row>
     <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>167</v>
@@ -9678,7 +9678,7 @@
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>168</v>
@@ -9689,7 +9689,7 @@
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>169</v>
@@ -9700,7 +9700,7 @@
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>170</v>
@@ -9711,7 +9711,7 @@
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>171</v>
@@ -9722,7 +9722,7 @@
     </row>
     <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>172</v>
@@ -9744,18 +9744,18 @@
     </row>
     <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B110" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="B110" s="0" t="s">
-        <v>175</v>
-      </c>
       <c r="C110" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>176</v>
@@ -9766,29 +9766,29 @@
     </row>
     <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>42</v>
+        <v>177</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>42</v>
+        <v>177</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>178</v>
+        <v>42</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>178</v>
+        <v>42</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B114" s="0" t="s">
         <v>179</v>
@@ -9799,7 +9799,7 @@
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B115" s="0" t="s">
         <v>180</v>
@@ -9810,7 +9810,7 @@
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B116" s="0" t="s">
         <v>181</v>
@@ -9821,7 +9821,7 @@
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>182</v>
@@ -9832,7 +9832,7 @@
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B118" s="0" t="s">
         <v>183</v>
@@ -9843,7 +9843,7 @@
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>184</v>
@@ -9854,7 +9854,7 @@
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>185</v>
@@ -9865,7 +9865,7 @@
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>186</v>
@@ -9876,7 +9876,7 @@
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B122" s="0" t="s">
         <v>187</v>
@@ -9887,51 +9887,51 @@
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>42</v>
+        <v>188</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>42</v>
+        <v>188</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>189</v>
+        <v>98</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>189</v>
+        <v>98</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B127" s="0" t="s">
         <v>190</v>
@@ -9942,7 +9942,7 @@
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>191</v>
@@ -9953,7 +9953,7 @@
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>192</v>
@@ -9964,40 +9964,40 @@
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>82</v>
+        <v>193</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>194</v>
+        <v>42</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>194</v>
+        <v>42</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B133" s="0" t="s">
         <v>195</v>
@@ -10008,40 +10008,40 @@
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>82</v>
+        <v>196</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>82</v>
+        <v>196</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>197</v>
+        <v>85</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>197</v>
+        <v>85</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B137" s="0" t="s">
         <v>198</v>
@@ -10052,51 +10052,51 @@
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>42</v>
+        <v>199</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>42</v>
+        <v>199</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>199</v>
+        <v>42</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>199</v>
+        <v>42</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>85</v>
+        <v>200</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>85</v>
+        <v>200</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>201</v>
+        <v>85</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>201</v>
+        <v>85</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B142" s="0" t="s">
         <v>202</v>
@@ -10107,7 +10107,7 @@
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B143" s="0" t="s">
         <v>203</v>
@@ -10118,7 +10118,7 @@
     </row>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B144" s="0" t="s">
         <v>204</v>
@@ -10129,29 +10129,29 @@
     </row>
     <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>42</v>
+        <v>205</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>42</v>
+        <v>205</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>206</v>
+        <v>42</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>206</v>
+        <v>42</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B147" s="0" t="s">
         <v>207</v>
@@ -10162,7 +10162,7 @@
     </row>
     <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B148" s="0" t="s">
         <v>208</v>
@@ -10173,29 +10173,29 @@
     </row>
     <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>42</v>
+        <v>209</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>42</v>
+        <v>209</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>210</v>
+        <v>42</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>210</v>
+        <v>42</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B151" s="0" t="s">
         <v>211</v>
@@ -10206,7 +10206,7 @@
     </row>
     <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
       <c r="B152" s="0" t="s">
         <v>212</v>
@@ -10341,26 +10341,26 @@
         <v>44</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>42</v>
+        <v>224</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>42</v>
+        <v>224</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>224</v>
+        <v>44</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>225</v>
+        <v>42</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>225</v>
+        <v>42</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B166" s="0" t="s">
         <v>226</v>
@@ -10371,139 +10371,139 @@
     </row>
     <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B167" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="B167" s="0" t="s">
-        <v>228</v>
-      </c>
       <c r="C167" s="0" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>132</v>
+        <v>229</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>132</v>
+        <v>229</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>229</v>
+        <v>132</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>229</v>
+        <v>132</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>133</v>
+        <v>230</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>133</v>
+        <v>230</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>134</v>
+        <v>231</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>134</v>
+        <v>231</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>231</v>
+        <v>134</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>231</v>
+        <v>134</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>135</v>
+        <v>232</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>230</v>
+        <v>98</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>230</v>
+        <v>98</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B179" s="0" t="s">
         <v>234</v>
@@ -10514,7 +10514,7 @@
     </row>
     <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B180" s="0" t="s">
         <v>235</v>
@@ -10525,7 +10525,7 @@
     </row>
     <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B181" s="0" t="s">
         <v>236</v>
@@ -10536,7 +10536,7 @@
     </row>
     <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B182" s="0" t="s">
         <v>237</v>
@@ -10547,29 +10547,29 @@
     </row>
     <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>133</v>
+        <v>238</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>133</v>
+        <v>238</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>238</v>
+        <v>133</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>238</v>
+        <v>133</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B185" s="0" t="s">
         <v>239</v>
@@ -10580,29 +10580,29 @@
     </row>
     <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>98</v>
+        <v>240</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>98</v>
+        <v>240</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>241</v>
+        <v>98</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>241</v>
+        <v>98</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B188" s="0" t="s">
         <v>242</v>
@@ -10613,7 +10613,7 @@
     </row>
     <row r="189" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B189" s="0" t="s">
         <v>243</v>
@@ -10624,7 +10624,7 @@
     </row>
     <row r="190" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B190" s="0" t="s">
         <v>244</v>
@@ -10635,18 +10635,18 @@
     </row>
     <row r="191" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B191" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="B191" s="0" t="s">
-        <v>246</v>
-      </c>
       <c r="C191" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B192" s="0" t="s">
         <v>247</v>
@@ -10657,7 +10657,7 @@
     </row>
     <row r="193" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B193" s="0" t="s">
         <v>248</v>
@@ -10668,7 +10668,7 @@
     </row>
     <row r="194" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B194" s="0" t="s">
         <v>249</v>
@@ -10679,7 +10679,7 @@
     </row>
     <row r="195" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B195" s="0" t="s">
         <v>250</v>
@@ -10690,7 +10690,7 @@
     </row>
     <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B196" s="0" t="s">
         <v>251</v>
@@ -10701,7 +10701,7 @@
     </row>
     <row r="197" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B197" s="0" t="s">
         <v>252</v>
@@ -10712,7 +10712,7 @@
     </row>
     <row r="198" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B198" s="0" t="s">
         <v>253</v>
@@ -10723,7 +10723,7 @@
     </row>
     <row r="199" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B199" s="0" t="s">
         <v>254</v>
@@ -10734,7 +10734,7 @@
     </row>
     <row r="200" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B200" s="0" t="s">
         <v>255</v>
@@ -10745,7 +10745,7 @@
     </row>
     <row r="201" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B201" s="0" t="s">
         <v>256</v>
@@ -10756,7 +10756,7 @@
     </row>
     <row r="202" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B202" s="0" t="s">
         <v>257</v>
@@ -10767,7 +10767,7 @@
     </row>
     <row r="203" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B203" s="0" t="s">
         <v>258</v>
@@ -10778,24 +10778,24 @@
     </row>
     <row r="204" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>98</v>
+        <v>259</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>68</v>
+        <v>246</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>259</v>
+        <v>98</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>259</v>
+        <v>98</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10811,18 +10811,18 @@
     </row>
     <row r="207" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B207" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="B207" s="0" t="s">
-        <v>262</v>
-      </c>
       <c r="C207" s="0" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B208" s="0" t="s">
         <v>263</v>
@@ -10833,7 +10833,7 @@
     </row>
     <row r="209" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B209" s="0" t="s">
         <v>264</v>
@@ -10844,24 +10844,24 @@
     </row>
     <row r="210" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>42</v>
+        <v>154</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>42</v>
+        <v>154</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>266</v>
+        <v>42</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>266</v>
+        <v>42</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10869,10 +10869,10 @@
         <v>265</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10880,10 +10880,10 @@
         <v>265</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10891,21 +10891,21 @@
         <v>265</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10913,10 +10913,10 @@
         <v>270</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10924,10 +10924,10 @@
         <v>270</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10935,10 +10935,10 @@
         <v>270</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10946,21 +10946,21 @@
         <v>270</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10968,10 +10968,10 @@
         <v>276</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10979,10 +10979,10 @@
         <v>276</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10990,10 +10990,10 @@
         <v>276</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11001,21 +11001,21 @@
         <v>276</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11023,10 +11023,10 @@
         <v>277</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11034,10 +11034,10 @@
         <v>277</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11045,21 +11045,21 @@
         <v>277</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11067,10 +11067,10 @@
         <v>278</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C230" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11078,10 +11078,10 @@
         <v>278</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11089,10 +11089,10 @@
         <v>278</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C232" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11100,10 +11100,10 @@
         <v>278</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C233" s="0" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11111,10 +11111,10 @@
         <v>278</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C234" s="0" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11122,10 +11122,10 @@
         <v>278</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C235" s="0" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11133,10 +11133,10 @@
         <v>278</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11144,10 +11144,10 @@
         <v>278</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C237" s="0" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11155,10 +11155,10 @@
         <v>278</v>
       </c>
       <c r="B238" s="0" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C238" s="0" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11166,21 +11166,21 @@
         <v>278</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>152</v>
+        <v>288</v>
       </c>
       <c r="C239" s="0" t="s">
-        <v>152</v>
+        <v>288</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>290</v>
+        <v>152</v>
       </c>
       <c r="C240" s="0" t="s">
-        <v>290</v>
+        <v>152</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11188,10 +11188,10 @@
         <v>289</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C241" s="0" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11199,10 +11199,10 @@
         <v>289</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11210,10 +11210,10 @@
         <v>289</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C243" s="0" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11221,10 +11221,10 @@
         <v>289</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C244" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11232,10 +11232,10 @@
         <v>289</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C245" s="0" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11243,10 +11243,10 @@
         <v>289</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11254,10 +11254,10 @@
         <v>289</v>
       </c>
       <c r="B247" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C247" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11265,10 +11265,10 @@
         <v>289</v>
       </c>
       <c r="B248" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C248" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11276,10 +11276,10 @@
         <v>289</v>
       </c>
       <c r="B249" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C249" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11287,10 +11287,10 @@
         <v>289</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C250" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11298,10 +11298,10 @@
         <v>289</v>
       </c>
       <c r="B251" s="0" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C251" s="0" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11309,10 +11309,10 @@
         <v>289</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C252" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11320,10 +11320,10 @@
         <v>289</v>
       </c>
       <c r="B253" s="0" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C253" s="0" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11331,10 +11331,10 @@
         <v>289</v>
       </c>
       <c r="B254" s="0" t="s">
-        <v>42</v>
+        <v>303</v>
       </c>
       <c r="C254" s="0" t="s">
-        <v>42</v>
+        <v>303</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11342,10 +11342,10 @@
         <v>289</v>
       </c>
       <c r="B255" s="0" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="C255" s="0" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11353,10 +11353,10 @@
         <v>289</v>
       </c>
       <c r="B256" s="0" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C256" s="0" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11364,21 +11364,21 @@
         <v>289</v>
       </c>
       <c r="B257" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C257" s="0" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="B258" s="0" t="n">
-        <v>1</v>
+        <v>289</v>
+      </c>
+      <c r="B258" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="C258" s="0" t="s">
-        <v>305</v>
+        <v>82</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11386,10 +11386,10 @@
         <v>304</v>
       </c>
       <c r="B259" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C259" s="0" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11397,10 +11397,10 @@
         <v>304</v>
       </c>
       <c r="B260" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C260" s="0" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11408,10 +11408,10 @@
         <v>304</v>
       </c>
       <c r="B261" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11419,10 +11419,10 @@
         <v>304</v>
       </c>
       <c r="B262" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C262" s="0" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11430,10 +11430,10 @@
         <v>304</v>
       </c>
       <c r="B263" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C263" s="0" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11441,10 +11441,10 @@
         <v>304</v>
       </c>
       <c r="B264" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C264" s="0" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11452,10 +11452,10 @@
         <v>304</v>
       </c>
       <c r="B265" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C265" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11463,10 +11463,10 @@
         <v>304</v>
       </c>
       <c r="B266" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C266" s="0" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11474,10 +11474,10 @@
         <v>304</v>
       </c>
       <c r="B267" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C267" s="0" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11485,10 +11485,10 @@
         <v>304</v>
       </c>
       <c r="B268" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C268" s="0" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11496,10 +11496,10 @@
         <v>304</v>
       </c>
       <c r="B269" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C269" s="0" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11507,10 +11507,10 @@
         <v>304</v>
       </c>
       <c r="B270" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C270" s="0" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11518,10 +11518,10 @@
         <v>304</v>
       </c>
       <c r="B271" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C271" s="0" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11529,10 +11529,10 @@
         <v>304</v>
       </c>
       <c r="B272" s="0" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C272" s="0" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11540,10 +11540,10 @@
         <v>304</v>
       </c>
       <c r="B273" s="0" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C273" s="0" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11551,10 +11551,10 @@
         <v>304</v>
       </c>
       <c r="B274" s="0" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C274" s="0" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11562,10 +11562,10 @@
         <v>304</v>
       </c>
       <c r="B275" s="0" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C275" s="0" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11573,10 +11573,10 @@
         <v>304</v>
       </c>
       <c r="B276" s="0" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C276" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11584,10 +11584,10 @@
         <v>304</v>
       </c>
       <c r="B277" s="0" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C277" s="0" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11595,10 +11595,10 @@
         <v>304</v>
       </c>
       <c r="B278" s="0" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C278" s="0" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11606,10 +11606,10 @@
         <v>304</v>
       </c>
       <c r="B279" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C279" s="0" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11617,10 +11617,10 @@
         <v>304</v>
       </c>
       <c r="B280" s="0" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C280" s="0" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11628,10 +11628,10 @@
         <v>304</v>
       </c>
       <c r="B281" s="0" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C281" s="0" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11639,10 +11639,10 @@
         <v>304</v>
       </c>
       <c r="B282" s="0" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C282" s="0" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11650,10 +11650,10 @@
         <v>304</v>
       </c>
       <c r="B283" s="0" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C283" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11661,10 +11661,10 @@
         <v>304</v>
       </c>
       <c r="B284" s="0" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C284" s="0" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11672,10 +11672,10 @@
         <v>304</v>
       </c>
       <c r="B285" s="0" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C285" s="0" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11683,10 +11683,10 @@
         <v>304</v>
       </c>
       <c r="B286" s="0" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C286" s="0" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11694,10 +11694,10 @@
         <v>304</v>
       </c>
       <c r="B287" s="0" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C287" s="0" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11705,21 +11705,21 @@
         <v>304</v>
       </c>
       <c r="B288" s="0" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C288" s="0" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="B289" s="0" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C289" s="0" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11727,10 +11727,10 @@
         <v>336</v>
       </c>
       <c r="B290" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C290" s="0" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11738,10 +11738,10 @@
         <v>336</v>
       </c>
       <c r="B291" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C291" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11749,10 +11749,10 @@
         <v>336</v>
       </c>
       <c r="B292" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C292" s="0" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11760,10 +11760,10 @@
         <v>336</v>
       </c>
       <c r="B293" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C293" s="0" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11771,10 +11771,10 @@
         <v>336</v>
       </c>
       <c r="B294" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C294" s="0" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11782,10 +11782,10 @@
         <v>336</v>
       </c>
       <c r="B295" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C295" s="0" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11793,10 +11793,10 @@
         <v>336</v>
       </c>
       <c r="B296" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C296" s="0" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11804,10 +11804,10 @@
         <v>336</v>
       </c>
       <c r="B297" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C297" s="0" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11815,10 +11815,10 @@
         <v>336</v>
       </c>
       <c r="B298" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C298" s="0" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11826,10 +11826,10 @@
         <v>336</v>
       </c>
       <c r="B299" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C299" s="0" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11837,21 +11837,21 @@
         <v>336</v>
       </c>
       <c r="B300" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C300" s="0" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="B301" s="0" t="n">
-        <v>2021</v>
+        <v>12</v>
       </c>
       <c r="C301" s="0" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11859,10 +11859,10 @@
         <v>349</v>
       </c>
       <c r="B302" s="0" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C302" s="0" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11870,10 +11870,10 @@
         <v>349</v>
       </c>
       <c r="B303" s="0" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C303" s="0" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11881,10 +11881,10 @@
         <v>349</v>
       </c>
       <c r="B304" s="0" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C304" s="0" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11892,10 +11892,10 @@
         <v>349</v>
       </c>
       <c r="B305" s="0" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C305" s="0" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11903,10 +11903,10 @@
         <v>349</v>
       </c>
       <c r="B306" s="0" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="C306" s="0" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11914,10 +11914,10 @@
         <v>349</v>
       </c>
       <c r="B307" s="0" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="C307" s="0" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11925,10 +11925,10 @@
         <v>349</v>
       </c>
       <c r="B308" s="0" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="C308" s="0" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11936,10 +11936,10 @@
         <v>349</v>
       </c>
       <c r="B309" s="0" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="C309" s="0" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11947,10 +11947,10 @@
         <v>349</v>
       </c>
       <c r="B310" s="0" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="C310" s="0" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11958,10 +11958,10 @@
         <v>349</v>
       </c>
       <c r="B311" s="0" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="C311" s="0" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11969,10 +11969,10 @@
         <v>349</v>
       </c>
       <c r="B312" s="0" t="n">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="C312" s="0" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11980,10 +11980,10 @@
         <v>349</v>
       </c>
       <c r="B313" s="0" t="n">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="C313" s="0" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11991,10 +11991,10 @@
         <v>349</v>
       </c>
       <c r="B314" s="0" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="C314" s="0" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12002,10 +12002,10 @@
         <v>349</v>
       </c>
       <c r="B315" s="0" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="C315" s="0" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12013,10 +12013,10 @@
         <v>349</v>
       </c>
       <c r="B316" s="0" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="C316" s="0" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12024,10 +12024,10 @@
         <v>349</v>
       </c>
       <c r="B317" s="0" t="n">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="C317" s="0" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12035,10 +12035,10 @@
         <v>349</v>
       </c>
       <c r="B318" s="0" t="n">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="C318" s="0" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12046,10 +12046,10 @@
         <v>349</v>
       </c>
       <c r="B319" s="0" t="n">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="C319" s="0" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12057,10 +12057,10 @@
         <v>349</v>
       </c>
       <c r="B320" s="0" t="n">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="C320" s="0" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12068,10 +12068,10 @@
         <v>349</v>
       </c>
       <c r="B321" s="0" t="n">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12079,10 +12079,10 @@
         <v>349</v>
       </c>
       <c r="B322" s="0" t="n">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12090,10 +12090,10 @@
         <v>349</v>
       </c>
       <c r="B323" s="0" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12101,10 +12101,10 @@
         <v>349</v>
       </c>
       <c r="B324" s="0" t="n">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="C324" s="0" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12112,10 +12112,10 @@
         <v>349</v>
       </c>
       <c r="B325" s="0" t="n">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="C325" s="0" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12123,10 +12123,10 @@
         <v>349</v>
       </c>
       <c r="B326" s="0" t="n">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="C326" s="0" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12134,10 +12134,10 @@
         <v>349</v>
       </c>
       <c r="B327" s="0" t="n">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="C327" s="0" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12145,10 +12145,10 @@
         <v>349</v>
       </c>
       <c r="B328" s="0" t="n">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="C328" s="0" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12156,10 +12156,10 @@
         <v>349</v>
       </c>
       <c r="B329" s="0" t="n">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="C329" s="0" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12167,10 +12167,10 @@
         <v>349</v>
       </c>
       <c r="B330" s="0" t="n">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="C330" s="0" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12178,10 +12178,10 @@
         <v>349</v>
       </c>
       <c r="B331" s="0" t="n">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="C331" s="0" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12189,10 +12189,10 @@
         <v>349</v>
       </c>
       <c r="B332" s="0" t="n">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="C332" s="0" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12200,10 +12200,10 @@
         <v>349</v>
       </c>
       <c r="B333" s="0" t="n">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="C333" s="0" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12211,10 +12211,10 @@
         <v>349</v>
       </c>
       <c r="B334" s="0" t="n">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="C334" s="0" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12222,10 +12222,10 @@
         <v>349</v>
       </c>
       <c r="B335" s="0" t="n">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12233,10 +12233,10 @@
         <v>349</v>
       </c>
       <c r="B336" s="0" t="n">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12244,10 +12244,10 @@
         <v>349</v>
       </c>
       <c r="B337" s="0" t="n">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12255,10 +12255,10 @@
         <v>349</v>
       </c>
       <c r="B338" s="0" t="n">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="C338" s="0" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12266,10 +12266,10 @@
         <v>349</v>
       </c>
       <c r="B339" s="0" t="n">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="C339" s="0" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12277,10 +12277,10 @@
         <v>349</v>
       </c>
       <c r="B340" s="0" t="n">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12288,10 +12288,10 @@
         <v>349</v>
       </c>
       <c r="B341" s="0" t="n">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12299,10 +12299,10 @@
         <v>349</v>
       </c>
       <c r="B342" s="0" t="n">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="C342" s="0" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12310,10 +12310,10 @@
         <v>349</v>
       </c>
       <c r="B343" s="0" t="n">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12321,10 +12321,10 @@
         <v>349</v>
       </c>
       <c r="B344" s="0" t="n">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="C344" s="0" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12332,10 +12332,10 @@
         <v>349</v>
       </c>
       <c r="B345" s="0" t="n">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12343,10 +12343,10 @@
         <v>349</v>
       </c>
       <c r="B346" s="0" t="n">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12354,10 +12354,10 @@
         <v>349</v>
       </c>
       <c r="B347" s="0" t="n">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="C347" s="0" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12365,10 +12365,10 @@
         <v>349</v>
       </c>
       <c r="B348" s="0" t="n">
-        <v>1974</v>
+        <v>1975</v>
       </c>
       <c r="C348" s="0" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12376,10 +12376,10 @@
         <v>349</v>
       </c>
       <c r="B349" s="0" t="n">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12387,10 +12387,10 @@
         <v>349</v>
       </c>
       <c r="B350" s="0" t="n">
-        <v>1972</v>
+        <v>1973</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12398,10 +12398,10 @@
         <v>349</v>
       </c>
       <c r="B351" s="0" t="n">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12409,10 +12409,10 @@
         <v>349</v>
       </c>
       <c r="B352" s="0" t="n">
-        <v>1970</v>
+        <v>1971</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12420,10 +12420,10 @@
         <v>349</v>
       </c>
       <c r="B353" s="0" t="n">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="C353" s="0" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12431,10 +12431,10 @@
         <v>349</v>
       </c>
       <c r="B354" s="0" t="n">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="C354" s="0" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12442,10 +12442,10 @@
         <v>349</v>
       </c>
       <c r="B355" s="0" t="n">
-        <v>1967</v>
+        <v>1968</v>
       </c>
       <c r="C355" s="0" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12453,10 +12453,10 @@
         <v>349</v>
       </c>
       <c r="B356" s="0" t="n">
-        <v>1966</v>
+        <v>1967</v>
       </c>
       <c r="C356" s="0" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12464,10 +12464,10 @@
         <v>349</v>
       </c>
       <c r="B357" s="0" t="n">
-        <v>1965</v>
+        <v>1966</v>
       </c>
       <c r="C357" s="0" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12475,10 +12475,10 @@
         <v>349</v>
       </c>
       <c r="B358" s="0" t="n">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12486,10 +12486,10 @@
         <v>349</v>
       </c>
       <c r="B359" s="0" t="n">
-        <v>1963</v>
+        <v>1964</v>
       </c>
       <c r="C359" s="0" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12497,10 +12497,10 @@
         <v>349</v>
       </c>
       <c r="B360" s="0" t="n">
-        <v>1962</v>
+        <v>1963</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12508,10 +12508,10 @@
         <v>349</v>
       </c>
       <c r="B361" s="0" t="n">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12519,10 +12519,10 @@
         <v>349</v>
       </c>
       <c r="B362" s="0" t="n">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12530,10 +12530,10 @@
         <v>349</v>
       </c>
       <c r="B363" s="0" t="n">
-        <v>1959</v>
+        <v>1960</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12541,10 +12541,10 @@
         <v>349</v>
       </c>
       <c r="B364" s="0" t="n">
-        <v>1958</v>
+        <v>1959</v>
       </c>
       <c r="C364" s="0" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12552,10 +12552,10 @@
         <v>349</v>
       </c>
       <c r="B365" s="0" t="n">
-        <v>1957</v>
+        <v>1958</v>
       </c>
       <c r="C365" s="0" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12563,10 +12563,10 @@
         <v>349</v>
       </c>
       <c r="B366" s="0" t="n">
-        <v>1956</v>
+        <v>1957</v>
       </c>
       <c r="C366" s="0" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12574,10 +12574,10 @@
         <v>349</v>
       </c>
       <c r="B367" s="0" t="n">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="C367" s="0" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12585,10 +12585,10 @@
         <v>349</v>
       </c>
       <c r="B368" s="0" t="n">
-        <v>1954</v>
+        <v>1955</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12596,10 +12596,10 @@
         <v>349</v>
       </c>
       <c r="B369" s="0" t="n">
-        <v>1953</v>
+        <v>1954</v>
       </c>
       <c r="C369" s="0" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12607,10 +12607,10 @@
         <v>349</v>
       </c>
       <c r="B370" s="0" t="n">
-        <v>1952</v>
+        <v>1953</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12618,10 +12618,10 @@
         <v>349</v>
       </c>
       <c r="B371" s="0" t="n">
-        <v>1951</v>
+        <v>1952</v>
       </c>
       <c r="C371" s="0" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12629,10 +12629,10 @@
         <v>349</v>
       </c>
       <c r="B372" s="0" t="n">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12640,10 +12640,10 @@
         <v>349</v>
       </c>
       <c r="B373" s="0" t="n">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12651,10 +12651,10 @@
         <v>349</v>
       </c>
       <c r="B374" s="0" t="n">
-        <v>1948</v>
+        <v>1949</v>
       </c>
       <c r="C374" s="0" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12662,10 +12662,10 @@
         <v>349</v>
       </c>
       <c r="B375" s="0" t="n">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12673,10 +12673,10 @@
         <v>349</v>
       </c>
       <c r="B376" s="0" t="n">
-        <v>1946</v>
+        <v>1947</v>
       </c>
       <c r="C376" s="0" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12684,10 +12684,10 @@
         <v>349</v>
       </c>
       <c r="B377" s="0" t="n">
-        <v>1945</v>
+        <v>1946</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12695,10 +12695,10 @@
         <v>349</v>
       </c>
       <c r="B378" s="0" t="n">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12706,10 +12706,10 @@
         <v>349</v>
       </c>
       <c r="B379" s="0" t="n">
-        <v>1943</v>
+        <v>1944</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12717,10 +12717,10 @@
         <v>349</v>
       </c>
       <c r="B380" s="0" t="n">
-        <v>1942</v>
+        <v>1943</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12728,10 +12728,10 @@
         <v>349</v>
       </c>
       <c r="B381" s="0" t="n">
-        <v>1941</v>
+        <v>1942</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12739,10 +12739,10 @@
         <v>349</v>
       </c>
       <c r="B382" s="0" t="n">
-        <v>1940</v>
+        <v>1941</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12750,10 +12750,10 @@
         <v>349</v>
       </c>
       <c r="B383" s="0" t="n">
-        <v>1939</v>
+        <v>1940</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12761,10 +12761,10 @@
         <v>349</v>
       </c>
       <c r="B384" s="0" t="n">
-        <v>1938</v>
+        <v>1939</v>
       </c>
       <c r="C384" s="0" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12772,10 +12772,10 @@
         <v>349</v>
       </c>
       <c r="B385" s="0" t="n">
-        <v>1937</v>
+        <v>1938</v>
       </c>
       <c r="C385" s="0" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12783,10 +12783,10 @@
         <v>349</v>
       </c>
       <c r="B386" s="0" t="n">
-        <v>1936</v>
+        <v>1937</v>
       </c>
       <c r="C386" s="0" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12794,10 +12794,10 @@
         <v>349</v>
       </c>
       <c r="B387" s="0" t="n">
-        <v>1935</v>
+        <v>1936</v>
       </c>
       <c r="C387" s="0" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12805,10 +12805,10 @@
         <v>349</v>
       </c>
       <c r="B388" s="0" t="n">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="C388" s="0" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12816,10 +12816,10 @@
         <v>349</v>
       </c>
       <c r="B389" s="0" t="n">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="C389" s="0" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12827,10 +12827,10 @@
         <v>349</v>
       </c>
       <c r="B390" s="0" t="n">
-        <v>1932</v>
+        <v>1933</v>
       </c>
       <c r="C390" s="0" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12838,10 +12838,10 @@
         <v>349</v>
       </c>
       <c r="B391" s="0" t="n">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="C391" s="0" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12849,10 +12849,10 @@
         <v>349</v>
       </c>
       <c r="B392" s="0" t="n">
-        <v>1930</v>
+        <v>1931</v>
       </c>
       <c r="C392" s="0" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12860,10 +12860,10 @@
         <v>349</v>
       </c>
       <c r="B393" s="0" t="n">
-        <v>1929</v>
+        <v>1930</v>
       </c>
       <c r="C393" s="0" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12871,10 +12871,10 @@
         <v>349</v>
       </c>
       <c r="B394" s="0" t="n">
-        <v>1928</v>
+        <v>1929</v>
       </c>
       <c r="C394" s="0" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12882,10 +12882,10 @@
         <v>349</v>
       </c>
       <c r="B395" s="0" t="n">
-        <v>1927</v>
+        <v>1928</v>
       </c>
       <c r="C395" s="0" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12893,10 +12893,10 @@
         <v>349</v>
       </c>
       <c r="B396" s="0" t="n">
-        <v>1926</v>
+        <v>1927</v>
       </c>
       <c r="C396" s="0" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12904,10 +12904,10 @@
         <v>349</v>
       </c>
       <c r="B397" s="0" t="n">
-        <v>1925</v>
+        <v>1926</v>
       </c>
       <c r="C397" s="0" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12915,10 +12915,10 @@
         <v>349</v>
       </c>
       <c r="B398" s="0" t="n">
-        <v>1924</v>
+        <v>1925</v>
       </c>
       <c r="C398" s="0" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12926,10 +12926,10 @@
         <v>349</v>
       </c>
       <c r="B399" s="0" t="n">
-        <v>1923</v>
+        <v>1924</v>
       </c>
       <c r="C399" s="0" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12937,10 +12937,10 @@
         <v>349</v>
       </c>
       <c r="B400" s="0" t="n">
-        <v>1922</v>
+        <v>1923</v>
       </c>
       <c r="C400" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12948,10 +12948,10 @@
         <v>349</v>
       </c>
       <c r="B401" s="0" t="n">
-        <v>1921</v>
+        <v>1922</v>
       </c>
       <c r="C401" s="0" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12959,13 +12959,23 @@
         <v>349</v>
       </c>
       <c r="B402" s="0" t="n">
+        <v>1921</v>
+      </c>
+      <c r="C402" s="0" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="403" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A403" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="B403" s="0" t="n">
         <v>1920</v>
       </c>
-      <c r="C402" s="0" t="s">
+      <c r="C403" s="0" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="403" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="404" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="405" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="406" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -13576,6 +13586,7 @@
     <row r="1011" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1012" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1013" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1014" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -13594,7 +13605,7 @@
   </sheetPr>
   <dimension ref="A1:Y760"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -14394,7 +14405,7 @@
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -14483,14 +14494,14 @@
         <v>478</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -14673,7 +14684,7 @@
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -14708,7 +14719,7 @@
       </c>
       <c r="D36" s="10"/>
       <c r="E36" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -14830,7 +14841,7 @@
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -15461,7 +15472,7 @@
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
@@ -15493,7 +15504,7 @@
       </c>
       <c r="D61" s="12"/>
       <c r="E61" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
@@ -15518,14 +15529,14 @@
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
@@ -15714,7 +15725,7 @@
       </c>
       <c r="D68" s="12"/>
       <c r="E68" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
@@ -15775,7 +15786,7 @@
       </c>
       <c r="D70" s="12"/>
       <c r="E70" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -15868,7 +15879,7 @@
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
@@ -15961,7 +15972,7 @@
       </c>
       <c r="D76" s="12"/>
       <c r="E76" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
@@ -16025,7 +16036,7 @@
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
@@ -16089,7 +16100,7 @@
       </c>
       <c r="D80" s="12"/>
       <c r="E80" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
@@ -16217,7 +16228,7 @@
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
@@ -16313,7 +16324,7 @@
       </c>
       <c r="D87" s="12"/>
       <c r="E87" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
@@ -31284,7 +31295,7 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -31348,7 +31359,7 @@
         <v>566</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>20210223001</v>
+        <v>20210224001</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32432,9 +32443,9 @@
   <dimension ref="A1:D506"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B505" activeCellId="0" sqref="B505"/>
+      <selection pane="bottomLeft" activeCell="D359" activeCellId="0" sqref="D359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -33314,7 +33325,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>744</v>
@@ -33328,7 +33339,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B65" s="13" t="s">
         <v>747</v>
@@ -33342,7 +33353,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>750</v>
@@ -33356,7 +33367,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="13" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>753</v>
@@ -33370,7 +33381,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="13" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>754</v>
@@ -33384,7 +33395,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="13" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>757</v>
@@ -33398,7 +33409,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>758</v>
@@ -33412,7 +33423,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>761</v>
@@ -33426,21 +33437,21 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C72" s="13" t="s">
         <v>764</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>765</v>
@@ -33454,7 +33465,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>768</v>
@@ -33468,10 +33479,10 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>771</v>
@@ -33482,7 +33493,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="13" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>773</v>
@@ -33496,7 +33507,7 @@
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="13" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>776</v>
@@ -33510,7 +33521,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="13" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>779</v>
@@ -33524,7 +33535,7 @@
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="13" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>782</v>
@@ -33538,7 +33549,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B80" s="13" t="s">
         <v>785</v>
@@ -33552,7 +33563,7 @@
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>788</v>
@@ -33566,7 +33577,7 @@
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="13" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>791</v>
@@ -33580,7 +33591,7 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B83" s="13" t="s">
         <v>794</v>
@@ -33594,10 +33605,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="13" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>797</v>
@@ -33608,10 +33619,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>799</v>
@@ -33622,10 +33633,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C86" s="13" t="s">
         <v>801</v>
@@ -33636,10 +33647,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C87" s="13" t="s">
         <v>803</v>
@@ -33650,10 +33661,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="13" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C88" s="13" t="s">
         <v>805</v>
@@ -33664,13 +33675,13 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D89" s="13" t="s">
         <v>807</v>
@@ -33678,10 +33689,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C90" s="13" t="s">
         <v>808</v>
@@ -33692,10 +33703,10 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C91" s="13" t="s">
         <v>810</v>
@@ -33706,10 +33717,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C92" s="13" t="s">
         <v>812</v>
@@ -33720,10 +33731,10 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C93" s="13" t="s">
         <v>814</v>
@@ -33734,10 +33745,10 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="13" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C94" s="13" t="s">
         <v>816</v>
@@ -33748,10 +33759,10 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C95" s="13" t="s">
         <v>818</v>
@@ -33762,10 +33773,10 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="13" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C96" s="13" t="s">
         <v>820</v>
@@ -33776,10 +33787,10 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="13" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C97" s="13" t="s">
         <v>822</v>
@@ -33790,7 +33801,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B98" s="13" t="s">
         <v>824</v>
@@ -33804,7 +33815,7 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="13" t="s">
         <v>827</v>
@@ -33818,7 +33829,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B100" s="13" t="s">
         <v>830</v>
@@ -33832,7 +33843,7 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="13" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B101" s="13" t="s">
         <v>833</v>
@@ -33846,7 +33857,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" s="13" t="s">
         <v>836</v>
@@ -33860,10 +33871,10 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C103" s="13" t="s">
         <v>839</v>
@@ -33874,10 +33885,10 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C104" s="13" t="s">
         <v>841</v>
@@ -33888,10 +33899,10 @@
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C105" s="13" t="s">
         <v>843</v>
@@ -33902,10 +33913,10 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="13" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C106" s="13" t="s">
         <v>845</v>
@@ -33916,10 +33927,10 @@
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C107" s="13" t="s">
         <v>847</v>
@@ -33930,10 +33941,10 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C108" s="13" t="s">
         <v>849</v>
@@ -33944,10 +33955,10 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C109" s="13" t="s">
         <v>851</v>
@@ -33958,7 +33969,7 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="13" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B110" s="13" t="s">
         <v>853</v>
@@ -33972,7 +33983,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B111" s="13" t="s">
         <v>856</v>
@@ -33986,7 +33997,7 @@
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B112" s="13" t="s">
         <v>859</v>
@@ -34000,7 +34011,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="13" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B113" s="13" t="s">
         <v>862</v>
@@ -34014,7 +34025,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B114" s="13" t="s">
         <v>865</v>
@@ -34028,7 +34039,7 @@
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="13" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B115" s="13" t="s">
         <v>868</v>
@@ -34042,7 +34053,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B116" s="13" t="s">
         <v>871</v>
@@ -34056,7 +34067,7 @@
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B117" s="13" t="s">
         <v>874</v>
@@ -34070,7 +34081,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="13" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B118" s="13" t="s">
         <v>877</v>
@@ -34084,7 +34095,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="13" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B119" s="13" t="s">
         <v>880</v>
@@ -34098,7 +34109,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="13" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B120" s="13" t="s">
         <v>883</v>
@@ -34112,7 +34123,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="13" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B121" s="13" t="s">
         <v>886</v>
@@ -34126,7 +34137,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="13" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B122" s="13" t="s">
         <v>889</v>
@@ -34140,7 +34151,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="13" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B123" s="13" t="s">
         <v>892</v>
@@ -34154,7 +34165,7 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="13" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B124" s="13" t="s">
         <v>895</v>
@@ -34168,7 +34179,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="13" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B125" s="13" t="s">
         <v>898</v>
@@ -34182,24 +34193,24 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C126" s="13" t="s">
         <v>901</v>
       </c>
       <c r="D126" s="13" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="13" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C127" s="13" t="s">
         <v>902</v>
@@ -34210,10 +34221,10 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C128" s="13" t="s">
         <v>904</v>
@@ -34224,7 +34235,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="13" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B129" s="13" t="s">
         <v>906</v>
@@ -34238,10 +34249,10 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="13" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>909</v>
@@ -34252,10 +34263,10 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="13" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C131" s="13" t="s">
         <v>911</v>
@@ -34266,7 +34277,7 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="13" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B132" s="13" t="s">
         <v>913</v>
@@ -34280,10 +34291,10 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C133" s="13" t="s">
         <v>916</v>
@@ -34294,10 +34305,10 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="13" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C134" s="13" t="s">
         <v>918</v>
@@ -34308,7 +34319,7 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="13" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B135" s="13" t="s">
         <v>920</v>
@@ -34322,7 +34333,7 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B136" s="13" t="s">
         <v>923</v>
@@ -34336,7 +34347,7 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="13" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B137" s="13" t="s">
         <v>926</v>
@@ -34350,7 +34361,7 @@
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="13" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B138" s="13" t="s">
         <v>929</v>
@@ -34364,7 +34375,7 @@
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="13" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B139" s="13" t="s">
         <v>932</v>
@@ -34378,7 +34389,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B140" s="13" t="s">
         <v>935</v>
@@ -34392,7 +34403,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="13" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B141" s="13" t="s">
         <v>938</v>
@@ -34406,7 +34417,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B142" s="13" t="s">
         <v>941</v>
@@ -34420,7 +34431,7 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B143" s="13" t="s">
         <v>944</v>
@@ -34434,7 +34445,7 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B144" s="13" t="s">
         <v>947</v>
@@ -34448,7 +34459,7 @@
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="13" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B145" s="13" t="s">
         <v>950</v>
@@ -34462,7 +34473,7 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="13" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B146" s="13" t="s">
         <v>953</v>
@@ -34476,7 +34487,7 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="13" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B147" s="13" t="s">
         <v>956</v>
@@ -34490,7 +34501,7 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="13" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B148" s="13" t="s">
         <v>959</v>
@@ -34504,7 +34515,7 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="13" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B149" s="13" t="s">
         <v>962</v>
@@ -34518,7 +34529,7 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="13" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B150" s="13" t="s">
         <v>965</v>
@@ -34532,7 +34543,7 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B151" s="13" t="s">
         <v>968</v>
@@ -34546,7 +34557,7 @@
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B152" s="13" t="s">
         <v>971</v>
@@ -34560,7 +34571,7 @@
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="13" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B153" s="13" t="s">
         <v>974</v>
@@ -34574,7 +34585,7 @@
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B154" s="13" t="s">
         <v>977</v>
@@ -34588,7 +34599,7 @@
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="13" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B155" s="13" t="s">
         <v>980</v>
@@ -34602,7 +34613,7 @@
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B156" s="13" t="s">
         <v>983</v>
@@ -34616,7 +34627,7 @@
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B157" s="13" t="s">
         <v>986</v>
@@ -37374,7 +37385,7 @@
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="13" t="s">
-        <v>264</v>
+        <v>154</v>
       </c>
       <c r="B357" s="13" t="s">
         <v>1253</v>

</xml_diff>

<commit_message>
Fix prompt for individual Q4 and Q5
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -4725,7 +4725,7 @@
     <t xml:space="preserve">ind_q4</t>
   </si>
   <si>
-    <t xml:space="preserve">4. Has this participant sign the informed consent?</t>
+    <t xml:space="preserve">4. Has this participant signed the informed consent?</t>
   </si>
   <si>
     <t xml:space="preserve">4. Este participante assinou o consentimento informado?</t>
@@ -4737,7 +4737,7 @@
     <t xml:space="preserve">ind_q5</t>
   </si>
   <si>
-    <t xml:space="preserve">5. Has this participant sign the assent form?</t>
+    <t xml:space="preserve">5. Has this participant signed the assent form?</t>
   </si>
   <si>
     <t xml:space="preserve">5.  O participante assinou o assentimento informado?</t>
@@ -5796,7 +5796,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.33984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.3515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -6847,7 +6847,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.33984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.3515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.67"/>
@@ -8336,7 +8336,7 @@
       <selection pane="bottomLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.33984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.3515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -13609,7 +13609,7 @@
       <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.33984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.3515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -31295,11 +31295,11 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.33984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.3515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.04"/>
@@ -32442,10 +32442,10 @@
   </sheetPr>
   <dimension ref="A1:D506"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A316" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A400" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D359" activeCellId="0" sqref="D359"/>
+      <selection pane="bottomLeft" activeCell="B447" activeCellId="0" sqref="B447"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Use text for months
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3472" uniqueCount="1798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3448" uniqueCount="1798">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -13599,7 +13599,7 @@
   </sheetPr>
   <dimension ref="A1:Y758"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -32378,10 +32378,10 @@
   </sheetPr>
   <dimension ref="A1:D506"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A325" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A366" activeCellId="0" sqref="A366"/>
+      <selection pane="bottomLeft" activeCell="C223" activeCellId="0" sqref="C223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35490,13 +35490,7 @@
         <v>337</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>1060</v>
-      </c>
-      <c r="C223" s="13" t="s">
-        <v>1060</v>
-      </c>
-      <c r="D223" s="13" t="s">
-        <v>1060</v>
+        <v>857</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35504,13 +35498,7 @@
         <v>338</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C224" s="13" t="s">
-        <v>1061</v>
-      </c>
-      <c r="D224" s="13" t="s">
-        <v>1061</v>
+        <v>860</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35518,13 +35506,7 @@
         <v>339</v>
       </c>
       <c r="B225" s="13" t="s">
-        <v>1062</v>
-      </c>
-      <c r="C225" s="13" t="s">
-        <v>1062</v>
-      </c>
-      <c r="D225" s="13" t="s">
-        <v>1062</v>
+        <v>863</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35532,13 +35514,7 @@
         <v>340</v>
       </c>
       <c r="B226" s="13" t="s">
-        <v>1063</v>
-      </c>
-      <c r="C226" s="13" t="s">
-        <v>1063</v>
-      </c>
-      <c r="D226" s="13" t="s">
-        <v>1063</v>
+        <v>866</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35546,13 +35522,7 @@
         <v>341</v>
       </c>
       <c r="B227" s="13" t="s">
-        <v>1064</v>
-      </c>
-      <c r="C227" s="13" t="s">
-        <v>1064</v>
-      </c>
-      <c r="D227" s="13" t="s">
-        <v>1064</v>
+        <v>869</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35560,13 +35530,7 @@
         <v>342</v>
       </c>
       <c r="B228" s="13" t="s">
-        <v>1065</v>
-      </c>
-      <c r="C228" s="13" t="s">
-        <v>1065</v>
-      </c>
-      <c r="D228" s="13" t="s">
-        <v>1065</v>
+        <v>872</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35574,13 +35538,7 @@
         <v>343</v>
       </c>
       <c r="B229" s="13" t="s">
-        <v>1066</v>
-      </c>
-      <c r="C229" s="13" t="s">
-        <v>1066</v>
-      </c>
-      <c r="D229" s="13" t="s">
-        <v>1066</v>
+        <v>875</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35588,13 +35546,7 @@
         <v>344</v>
       </c>
       <c r="B230" s="13" t="s">
-        <v>1067</v>
-      </c>
-      <c r="C230" s="13" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D230" s="13" t="s">
-        <v>1067</v>
+        <v>878</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35602,13 +35554,7 @@
         <v>345</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>1068</v>
-      </c>
-      <c r="C231" s="13" t="s">
-        <v>1068</v>
-      </c>
-      <c r="D231" s="13" t="s">
-        <v>1068</v>
+        <v>881</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35616,13 +35562,7 @@
         <v>346</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>1069</v>
-      </c>
-      <c r="C232" s="13" t="s">
-        <v>1069</v>
-      </c>
-      <c r="D232" s="13" t="s">
-        <v>1069</v>
+        <v>884</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35630,13 +35570,7 @@
         <v>347</v>
       </c>
       <c r="B233" s="13" t="s">
-        <v>1070</v>
-      </c>
-      <c r="C233" s="13" t="s">
-        <v>1070</v>
-      </c>
-      <c r="D233" s="13" t="s">
-        <v>1070</v>
+        <v>887</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35644,13 +35578,7 @@
         <v>348</v>
       </c>
       <c r="B234" s="13" t="s">
-        <v>1071</v>
-      </c>
-      <c r="C234" s="13" t="s">
-        <v>1071</v>
-      </c>
-      <c r="D234" s="13" t="s">
-        <v>1071</v>
+        <v>890</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Remove unused translation keys
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="1796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3442" uniqueCount="1792">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -3843,12 +3843,6 @@
     <t xml:space="preserve">Data da emigracão não pode ser no futuro &lt;br&gt; Data da emigracao não pode ser antes de Outubro de 2020</t>
   </si>
   <si>
-    <t xml:space="preserve">err_emigrate_date_multiple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You only need to identify one time (date OR enter an integer OR select 'Don't Know')</t>
-  </si>
-  <si>
     <t xml:space="preserve">death_va_note</t>
   </si>
   <si>
@@ -4948,12 +4942,6 @@
   </si>
   <si>
     <t xml:space="preserve">17b (i). [Ikiwa ndiyo] Matokeo ya kipimo cha malaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ind_q17bi.hint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indicate result</t>
   </si>
   <si>
     <t xml:space="preserve">ind_q17c</t>
@@ -5589,7 +5577,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5651,10 +5639,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5784,7 +5768,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -6831,11 +6815,11 @@
   </sheetPr>
   <dimension ref="A1:P1016"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.67"/>
@@ -8318,7 +8302,7 @@
       <selection pane="bottomLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -13591,7 +13575,7 @@
       <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -31223,7 +31207,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.04"/>
@@ -32364,12 +32348,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D506"/>
+  <dimension ref="A1:D504"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A416" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C223" activeCellId="0" sqref="C223"/>
+      <selection pane="bottomLeft" activeCell="A464" activeCellId="0" sqref="A464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37326,426 +37310,424 @@
       <c r="B363" s="13" t="s">
         <v>1273</v>
       </c>
-      <c r="C363" s="16"/>
-      <c r="D363" s="16"/>
+      <c r="C363" s="13" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D363" s="13" t="s">
+        <v>1275</v>
+      </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="13" t="s">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="B364" s="13" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
       <c r="C364" s="13" t="s">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="D364" s="13" t="s">
-        <v>1277</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="13" t="s">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="B365" s="13" t="s">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="C365" s="13" t="s">
-        <v>1280</v>
+        <v>1282</v>
       </c>
       <c r="D365" s="13" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="13" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="B366" s="13" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="C366" s="13" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="D366" s="13" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="13" t="s">
-        <v>1286</v>
+        <v>1288</v>
       </c>
       <c r="B367" s="13" t="s">
-        <v>1287</v>
-      </c>
-      <c r="C367" s="13" t="s">
-        <v>1288</v>
-      </c>
-      <c r="D367" s="13" t="s">
         <v>1289</v>
+      </c>
+      <c r="C367" s="15" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D367" s="15" t="s">
+        <v>1291</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="13" t="s">
-        <v>1290</v>
+        <v>1292</v>
       </c>
       <c r="B368" s="13" t="s">
-        <v>1291</v>
-      </c>
-      <c r="C368" s="15" t="s">
-        <v>1292</v>
-      </c>
-      <c r="D368" s="15" t="s">
         <v>1293</v>
+      </c>
+      <c r="C368" s="13" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D368" s="13" t="s">
+        <v>1295</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="13" t="s">
-        <v>1294</v>
+        <v>1296</v>
       </c>
       <c r="B369" s="13" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="C369" s="13" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="D369" s="13" t="s">
         <v>1297</v>
       </c>
     </row>
-    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="13" t="s">
         <v>1298</v>
       </c>
       <c r="B370" s="13" t="s">
         <v>1299</v>
       </c>
-      <c r="C370" s="13" t="s">
-        <v>1299</v>
-      </c>
-      <c r="D370" s="13" t="s">
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="371" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C370" s="15" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D370" s="15" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="13" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="B371" s="13" t="s">
-        <v>1301</v>
-      </c>
-      <c r="C371" s="15" t="s">
-        <v>1302</v>
-      </c>
-      <c r="D371" s="15" t="s">
         <v>1303</v>
+      </c>
+      <c r="C371" s="13" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D371" s="13" t="s">
+        <v>1305</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="13" t="s">
-        <v>1304</v>
+        <v>1306</v>
       </c>
       <c r="B372" s="13" t="s">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="C372" s="13" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
       <c r="D372" s="13" t="s">
-        <v>1307</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="13" t="s">
-        <v>1308</v>
+        <v>26</v>
       </c>
       <c r="B373" s="13" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="C373" s="13" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
       <c r="D373" s="13" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="13" t="s">
-        <v>26</v>
+        <v>1313</v>
       </c>
       <c r="B374" s="13" t="s">
-        <v>1312</v>
+        <v>1314</v>
       </c>
       <c r="C374" s="13" t="s">
-        <v>1313</v>
+        <v>1315</v>
       </c>
       <c r="D374" s="13" t="s">
-        <v>1314</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="13" t="s">
-        <v>1315</v>
+        <v>1317</v>
       </c>
       <c r="B375" s="13" t="s">
-        <v>1316</v>
+        <v>1318</v>
       </c>
       <c r="C375" s="13" t="s">
-        <v>1317</v>
+        <v>1319</v>
       </c>
       <c r="D375" s="13" t="s">
-        <v>1318</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="13" t="s">
-        <v>1319</v>
+        <v>1321</v>
       </c>
       <c r="B376" s="13" t="s">
-        <v>1320</v>
+        <v>1322</v>
       </c>
       <c r="C376" s="13" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
       <c r="D376" s="13" t="s">
-        <v>1322</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="13" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
       <c r="B377" s="13" t="s">
-        <v>1324</v>
+        <v>1326</v>
       </c>
       <c r="C377" s="13" t="s">
-        <v>1325</v>
+        <v>1327</v>
       </c>
       <c r="D377" s="13" t="s">
-        <v>1326</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="13" t="s">
-        <v>1327</v>
+        <v>1329</v>
       </c>
       <c r="B378" s="13" t="s">
-        <v>1328</v>
+        <v>1330</v>
       </c>
       <c r="C378" s="13" t="s">
-        <v>1329</v>
+        <v>1331</v>
       </c>
       <c r="D378" s="13" t="s">
-        <v>1330</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="13" t="s">
-        <v>1331</v>
+        <v>1333</v>
       </c>
       <c r="B379" s="13" t="s">
-        <v>1332</v>
+        <v>1334</v>
       </c>
       <c r="C379" s="13" t="s">
-        <v>1333</v>
+        <v>1335</v>
       </c>
       <c r="D379" s="13" t="s">
-        <v>1334</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="13" t="s">
-        <v>1335</v>
+        <v>1337</v>
       </c>
       <c r="B380" s="13" t="s">
-        <v>1336</v>
+        <v>1338</v>
       </c>
       <c r="C380" s="13" t="s">
-        <v>1337</v>
+        <v>1339</v>
       </c>
       <c r="D380" s="13" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="13" t="s">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="B381" s="13" t="s">
-        <v>1340</v>
-      </c>
-      <c r="C381" s="13" t="s">
-        <v>1341</v>
-      </c>
-      <c r="D381" s="13" t="s">
         <v>1342</v>
       </c>
-    </row>
-    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C381" s="15" t="s">
+        <v>1343</v>
+      </c>
+      <c r="D381" s="15" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="13" t="s">
-        <v>1343</v>
+        <v>1345</v>
       </c>
       <c r="B382" s="13" t="s">
-        <v>1344</v>
+        <v>1346</v>
       </c>
       <c r="C382" s="15" t="s">
-        <v>1345</v>
+        <v>1347</v>
       </c>
       <c r="D382" s="15" t="s">
-        <v>1346</v>
-      </c>
-    </row>
-    <row r="383" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="13" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B383" s="13" t="s">
         <v>1348</v>
       </c>
-      <c r="C383" s="15" t="s">
+    </row>
+    <row r="384" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B384" s="13" t="s">
         <v>1349</v>
       </c>
-      <c r="D383" s="15" t="s">
+      <c r="C384" s="15" t="s">
         <v>1350</v>
       </c>
-    </row>
-    <row r="385" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D384" s="15" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A385" s="13" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B385" s="13" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="C385" s="15" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D385" s="15" t="s">
-        <v>1353</v>
-      </c>
-    </row>
-    <row r="386" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B386" s="13" t="s">
-        <v>1354</v>
-      </c>
-      <c r="C386" s="15" t="s">
         <v>1355</v>
       </c>
-      <c r="D386" s="15" t="s">
+      <c r="C386" s="13" t="s">
         <v>1356</v>
+      </c>
+      <c r="D386" s="13" t="s">
+        <v>1357</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="13" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B387" s="13" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="C387" s="13" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
       <c r="D387" s="13" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="13" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B388" s="13" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="C388" s="13" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D388" s="13" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="13" t="s">
-        <v>50</v>
+        <v>1364</v>
       </c>
       <c r="B389" s="13" t="s">
-        <v>1363</v>
+        <v>1365</v>
       </c>
       <c r="C389" s="13" t="s">
-        <v>1364</v>
+        <v>1366</v>
       </c>
       <c r="D389" s="13" t="s">
-        <v>1365</v>
-      </c>
-    </row>
-    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="13" t="s">
-        <v>1366</v>
+        <v>1368</v>
       </c>
       <c r="B390" s="13" t="s">
-        <v>1367</v>
-      </c>
-      <c r="C390" s="13" t="s">
-        <v>1368</v>
-      </c>
-      <c r="D390" s="13" t="s">
         <v>1369</v>
+      </c>
+      <c r="C390" s="15" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D390" s="15" t="s">
+        <v>1371</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="13" t="s">
-        <v>1370</v>
+        <v>1372</v>
       </c>
       <c r="B391" s="13" t="s">
-        <v>1371</v>
+        <v>1373</v>
       </c>
       <c r="C391" s="15" t="s">
-        <v>1372</v>
+        <v>1374</v>
       </c>
       <c r="D391" s="15" t="s">
-        <v>1373</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="13" t="s">
-        <v>1374</v>
+        <v>1376</v>
       </c>
       <c r="B392" s="13" t="s">
-        <v>1375</v>
+        <v>1377</v>
       </c>
       <c r="C392" s="15" t="s">
-        <v>1376</v>
+        <v>1378</v>
       </c>
       <c r="D392" s="15" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="393" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="13" t="s">
-        <v>1378</v>
+        <v>1380</v>
       </c>
       <c r="B393" s="13" t="s">
-        <v>1379</v>
-      </c>
-      <c r="C393" s="15" t="s">
-        <v>1380</v>
-      </c>
-      <c r="D393" s="15" t="s">
         <v>1381</v>
+      </c>
+      <c r="C393" s="13" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D393" s="13" t="s">
+        <v>1383</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="13" t="s">
-        <v>1382</v>
+        <v>1384</v>
       </c>
       <c r="B394" s="13" t="s">
-        <v>1383</v>
-      </c>
-      <c r="C394" s="13" t="s">
-        <v>1384</v>
-      </c>
-      <c r="D394" s="13" t="s">
         <v>1385</v>
       </c>
     </row>
@@ -37757,303 +37739,309 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="13" t="s">
+    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A397" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B397" s="13" t="s">
         <v>1388</v>
       </c>
-      <c r="B396" s="13" t="s">
+      <c r="C397" s="13" t="s">
         <v>1389</v>
+      </c>
+      <c r="D397" s="13" t="s">
+        <v>1390</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="13" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B398" s="13" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="C398" s="13" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="D398" s="13" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="13" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B399" s="13" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="C399" s="13" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="D399" s="13" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="13" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B400" s="13" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="C400" s="13" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="D400" s="13" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="13" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B401" s="13" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="C401" s="13" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="D401" s="13" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B402" s="13" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="C402" s="13" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="D402" s="13" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B403" s="13" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="C403" s="13" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="D403" s="13" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="13" t="s">
-        <v>69</v>
+        <v>1409</v>
       </c>
       <c r="B404" s="13" t="s">
-        <v>1408</v>
+        <v>1410</v>
       </c>
       <c r="C404" s="13" t="s">
-        <v>1409</v>
+        <v>1411</v>
       </c>
       <c r="D404" s="13" t="s">
-        <v>1410</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="13" t="s">
-        <v>1411</v>
+        <v>1413</v>
       </c>
       <c r="B405" s="13" t="s">
-        <v>1412</v>
+        <v>1414</v>
       </c>
       <c r="C405" s="13" t="s">
-        <v>1413</v>
+        <v>1415</v>
       </c>
       <c r="D405" s="13" t="s">
-        <v>1414</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="13" t="s">
-        <v>1415</v>
+        <v>1417</v>
       </c>
       <c r="B406" s="13" t="s">
-        <v>1416</v>
+        <v>1418</v>
       </c>
       <c r="C406" s="13" t="s">
-        <v>1417</v>
+        <v>1419</v>
       </c>
       <c r="D406" s="13" t="s">
-        <v>1418</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="13" t="s">
-        <v>1419</v>
+        <v>1421</v>
       </c>
       <c r="B407" s="13" t="s">
-        <v>1420</v>
+        <v>1422</v>
       </c>
       <c r="C407" s="13" t="s">
-        <v>1421</v>
+        <v>1423</v>
       </c>
       <c r="D407" s="13" t="s">
-        <v>1422</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="13" t="s">
-        <v>1423</v>
+        <v>1425</v>
       </c>
       <c r="B408" s="13" t="s">
-        <v>1424</v>
+        <v>1426</v>
       </c>
       <c r="C408" s="13" t="s">
-        <v>1425</v>
+        <v>1427</v>
       </c>
       <c r="D408" s="13" t="s">
-        <v>1426</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="13" t="s">
-        <v>1427</v>
+        <v>1429</v>
       </c>
       <c r="B409" s="13" t="s">
-        <v>1428</v>
+        <v>1430</v>
       </c>
       <c r="C409" s="13" t="s">
-        <v>1429</v>
+        <v>1431</v>
       </c>
       <c r="D409" s="13" t="s">
-        <v>1430</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="13" t="s">
-        <v>1431</v>
+        <v>1433</v>
       </c>
       <c r="B410" s="13" t="s">
-        <v>1432</v>
+        <v>1434</v>
       </c>
       <c r="C410" s="13" t="s">
-        <v>1433</v>
+        <v>1435</v>
       </c>
       <c r="D410" s="13" t="s">
-        <v>1434</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="13" t="s">
-        <v>1435</v>
+        <v>1437</v>
       </c>
       <c r="B411" s="13" t="s">
-        <v>1436</v>
+        <v>1438</v>
       </c>
       <c r="C411" s="13" t="s">
-        <v>1437</v>
+        <v>1439</v>
       </c>
       <c r="D411" s="13" t="s">
-        <v>1438</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="13" t="s">
-        <v>1439</v>
+        <v>1441</v>
       </c>
       <c r="B412" s="13" t="s">
-        <v>1440</v>
+        <v>1442</v>
       </c>
       <c r="C412" s="13" t="s">
-        <v>1441</v>
+        <v>1443</v>
       </c>
       <c r="D412" s="13" t="s">
-        <v>1442</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="13" t="s">
-        <v>1443</v>
+        <v>1445</v>
       </c>
       <c r="B413" s="13" t="s">
-        <v>1444</v>
+        <v>1446</v>
       </c>
       <c r="C413" s="13" t="s">
-        <v>1445</v>
+        <v>1447</v>
       </c>
       <c r="D413" s="13" t="s">
-        <v>1446</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="13" t="s">
-        <v>1447</v>
+        <v>1449</v>
       </c>
       <c r="B414" s="13" t="s">
-        <v>1448</v>
+        <v>1450</v>
       </c>
       <c r="C414" s="13" t="s">
-        <v>1449</v>
+        <v>1451</v>
       </c>
       <c r="D414" s="13" t="s">
-        <v>1450</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="13" t="s">
-        <v>1451</v>
+        <v>1453</v>
       </c>
       <c r="B415" s="13" t="s">
-        <v>1452</v>
+        <v>1454</v>
       </c>
       <c r="C415" s="13" t="s">
-        <v>1453</v>
+        <v>1455</v>
       </c>
       <c r="D415" s="13" t="s">
-        <v>1454</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="13" t="s">
-        <v>1455</v>
+        <v>1457</v>
       </c>
       <c r="B416" s="13" t="s">
-        <v>1456</v>
+        <v>1458</v>
       </c>
       <c r="C416" s="13" t="s">
-        <v>1457</v>
+        <v>1459</v>
       </c>
       <c r="D416" s="13" t="s">
-        <v>1458</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="13" t="s">
-        <v>1459</v>
+        <v>1461</v>
       </c>
       <c r="B417" s="13" t="s">
-        <v>1460</v>
+        <v>1406</v>
       </c>
       <c r="C417" s="13" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="D417" s="13" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="13" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="B418" s="13" t="s">
-        <v>1408</v>
+        <v>1465</v>
       </c>
       <c r="C418" s="13" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="D418" s="13" t="s">
         <v>1465</v>
@@ -38067,1124 +38055,1130 @@
         <v>1467</v>
       </c>
       <c r="C419" s="13" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="D419" s="13" t="s">
-        <v>1467</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="13" t="s">
-        <v>1468</v>
+        <v>1470</v>
       </c>
       <c r="B420" s="13" t="s">
-        <v>1469</v>
+        <v>1471</v>
       </c>
       <c r="C420" s="13" t="s">
-        <v>1470</v>
+        <v>1472</v>
       </c>
       <c r="D420" s="13" t="s">
-        <v>1471</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="13" t="s">
-        <v>1472</v>
+        <v>1474</v>
       </c>
       <c r="B421" s="13" t="s">
-        <v>1473</v>
+        <v>1475</v>
       </c>
       <c r="C421" s="13" t="s">
-        <v>1474</v>
+        <v>1476</v>
       </c>
       <c r="D421" s="13" t="s">
-        <v>1475</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="13" t="s">
-        <v>1476</v>
+        <v>1478</v>
       </c>
       <c r="B422" s="13" t="s">
-        <v>1477</v>
+        <v>1479</v>
       </c>
       <c r="C422" s="13" t="s">
-        <v>1478</v>
+        <v>1480</v>
       </c>
       <c r="D422" s="13" t="s">
-        <v>1479</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="13" t="s">
-        <v>1480</v>
+        <v>1482</v>
       </c>
       <c r="B423" s="13" t="s">
-        <v>1481</v>
+        <v>1483</v>
       </c>
       <c r="C423" s="13" t="s">
-        <v>1482</v>
+        <v>1484</v>
       </c>
       <c r="D423" s="13" t="s">
-        <v>1483</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="13" t="s">
-        <v>1484</v>
+        <v>1486</v>
       </c>
       <c r="B424" s="13" t="s">
-        <v>1485</v>
+        <v>1487</v>
       </c>
       <c r="C424" s="13" t="s">
-        <v>1486</v>
+        <v>1488</v>
       </c>
       <c r="D424" s="13" t="s">
-        <v>1487</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="13" t="s">
-        <v>1488</v>
+        <v>1490</v>
       </c>
       <c r="B425" s="13" t="s">
-        <v>1489</v>
+        <v>1406</v>
       </c>
       <c r="C425" s="13" t="s">
-        <v>1490</v>
+        <v>1462</v>
       </c>
       <c r="D425" s="13" t="s">
-        <v>1491</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="13" t="s">
+        <v>1491</v>
+      </c>
+      <c r="B426" s="13" t="s">
         <v>1492</v>
       </c>
-      <c r="B426" s="13" t="s">
-        <v>1408</v>
-      </c>
       <c r="C426" s="13" t="s">
-        <v>1464</v>
+        <v>1493</v>
       </c>
       <c r="D426" s="13" t="s">
-        <v>1465</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="13" t="s">
-        <v>1493</v>
+        <v>1495</v>
       </c>
       <c r="B427" s="13" t="s">
-        <v>1494</v>
+        <v>1496</v>
       </c>
       <c r="C427" s="13" t="s">
-        <v>1495</v>
+        <v>1497</v>
       </c>
       <c r="D427" s="13" t="s">
-        <v>1496</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="13" t="s">
-        <v>1497</v>
+        <v>1499</v>
       </c>
       <c r="B428" s="13" t="s">
-        <v>1498</v>
+        <v>1500</v>
       </c>
       <c r="C428" s="13" t="s">
-        <v>1499</v>
+        <v>1501</v>
       </c>
       <c r="D428" s="13" t="s">
-        <v>1500</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="13" t="s">
-        <v>1501</v>
+        <v>1503</v>
       </c>
       <c r="B429" s="13" t="s">
-        <v>1502</v>
+        <v>1504</v>
       </c>
       <c r="C429" s="13" t="s">
-        <v>1503</v>
+        <v>1505</v>
       </c>
       <c r="D429" s="13" t="s">
-        <v>1504</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="13" t="s">
-        <v>1505</v>
+        <v>1507</v>
       </c>
       <c r="B430" s="13" t="s">
-        <v>1506</v>
+        <v>1508</v>
       </c>
       <c r="C430" s="13" t="s">
-        <v>1507</v>
+        <v>1509</v>
       </c>
       <c r="D430" s="13" t="s">
-        <v>1508</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="13" t="s">
-        <v>1509</v>
+        <v>1511</v>
       </c>
       <c r="B431" s="13" t="s">
-        <v>1510</v>
+        <v>1512</v>
       </c>
       <c r="C431" s="13" t="s">
-        <v>1511</v>
+        <v>1513</v>
       </c>
       <c r="D431" s="13" t="s">
-        <v>1512</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="13" t="s">
-        <v>1513</v>
+        <v>1515</v>
       </c>
       <c r="B432" s="13" t="s">
-        <v>1514</v>
+        <v>1516</v>
       </c>
       <c r="C432" s="13" t="s">
-        <v>1515</v>
+        <v>1517</v>
       </c>
       <c r="D432" s="13" t="s">
-        <v>1516</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="13" t="s">
-        <v>1517</v>
+        <v>1519</v>
       </c>
       <c r="B433" s="13" t="s">
-        <v>1518</v>
+        <v>1520</v>
       </c>
       <c r="C433" s="13" t="s">
-        <v>1519</v>
+        <v>1521</v>
       </c>
       <c r="D433" s="13" t="s">
-        <v>1520</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="13" t="s">
-        <v>1521</v>
+        <v>1523</v>
       </c>
       <c r="B434" s="13" t="s">
-        <v>1522</v>
+        <v>1524</v>
       </c>
       <c r="C434" s="13" t="s">
-        <v>1523</v>
+        <v>1525</v>
       </c>
       <c r="D434" s="13" t="s">
-        <v>1524</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="13" t="s">
-        <v>1525</v>
+        <v>1527</v>
       </c>
       <c r="B435" s="13" t="s">
-        <v>1526</v>
+        <v>1528</v>
       </c>
       <c r="C435" s="13" t="s">
-        <v>1527</v>
+        <v>1529</v>
       </c>
       <c r="D435" s="13" t="s">
-        <v>1528</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="13" t="s">
-        <v>1529</v>
+        <v>1531</v>
       </c>
       <c r="B436" s="13" t="s">
-        <v>1530</v>
+        <v>1532</v>
       </c>
       <c r="C436" s="13" t="s">
-        <v>1531</v>
+        <v>1533</v>
       </c>
       <c r="D436" s="13" t="s">
-        <v>1532</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="13" t="s">
-        <v>1533</v>
+        <v>1535</v>
       </c>
       <c r="B437" s="13" t="s">
-        <v>1534</v>
+        <v>1536</v>
       </c>
       <c r="C437" s="13" t="s">
-        <v>1535</v>
+        <v>1537</v>
       </c>
       <c r="D437" s="13" t="s">
-        <v>1536</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="13" t="s">
-        <v>1537</v>
+        <v>1539</v>
       </c>
       <c r="B438" s="13" t="s">
-        <v>1538</v>
+        <v>1540</v>
       </c>
       <c r="C438" s="13" t="s">
-        <v>1539</v>
+        <v>1541</v>
       </c>
       <c r="D438" s="13" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="13" t="s">
-        <v>1541</v>
-      </c>
-      <c r="B439" s="13" t="s">
         <v>1542</v>
       </c>
-      <c r="C439" s="13" t="s">
+    </row>
+    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A440" s="13" t="s">
         <v>1543</v>
       </c>
-      <c r="D439" s="13" t="s">
+      <c r="B440" s="13" t="s">
         <v>1544</v>
+      </c>
+      <c r="C440" s="13" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D440" s="13" t="s">
+        <v>1546</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="13" t="s">
-        <v>1545</v>
+        <v>1547</v>
       </c>
       <c r="B441" s="13" t="s">
-        <v>1546</v>
+        <v>1548</v>
       </c>
       <c r="C441" s="13" t="s">
-        <v>1547</v>
+        <v>1549</v>
       </c>
       <c r="D441" s="13" t="s">
-        <v>1548</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="13" t="s">
-        <v>1549</v>
+        <v>1551</v>
       </c>
       <c r="B442" s="13" t="s">
-        <v>1550</v>
+        <v>1552</v>
       </c>
       <c r="C442" s="13" t="s">
-        <v>1551</v>
+        <v>1553</v>
       </c>
       <c r="D442" s="13" t="s">
-        <v>1552</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="13" t="s">
-        <v>1553</v>
+        <v>1555</v>
       </c>
       <c r="B443" s="13" t="s">
-        <v>1554</v>
+        <v>1556</v>
       </c>
       <c r="C443" s="13" t="s">
-        <v>1555</v>
+        <v>1557</v>
       </c>
       <c r="D443" s="13" t="s">
-        <v>1556</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="13" t="s">
-        <v>1557</v>
+        <v>1559</v>
       </c>
       <c r="B444" s="13" t="s">
-        <v>1558</v>
+        <v>1560</v>
       </c>
       <c r="C444" s="13" t="s">
-        <v>1559</v>
+        <v>1561</v>
       </c>
       <c r="D444" s="13" t="s">
-        <v>1560</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="13" t="s">
-        <v>1561</v>
+        <v>1563</v>
       </c>
       <c r="B445" s="13" t="s">
-        <v>1562</v>
+        <v>1564</v>
       </c>
       <c r="C445" s="13" t="s">
-        <v>1563</v>
+        <v>1565</v>
       </c>
       <c r="D445" s="13" t="s">
-        <v>1564</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="13" t="s">
-        <v>1565</v>
+        <v>1567</v>
       </c>
       <c r="B446" s="13" t="s">
-        <v>1566</v>
+        <v>1568</v>
       </c>
       <c r="C446" s="13" t="s">
-        <v>1567</v>
+        <v>1569</v>
       </c>
       <c r="D446" s="13" t="s">
-        <v>1568</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="13" t="s">
-        <v>1569</v>
+        <v>1571</v>
       </c>
       <c r="B447" s="13" t="s">
-        <v>1570</v>
+        <v>1572</v>
       </c>
       <c r="C447" s="13" t="s">
-        <v>1571</v>
+        <v>1573</v>
       </c>
       <c r="D447" s="13" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="13" t="s">
-        <v>1573</v>
+        <v>1575</v>
       </c>
       <c r="B448" s="13" t="s">
-        <v>1574</v>
+        <v>1576</v>
       </c>
       <c r="C448" s="13" t="s">
-        <v>1575</v>
+        <v>1577</v>
       </c>
       <c r="D448" s="13" t="s">
-        <v>1576</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="13" t="s">
-        <v>1577</v>
+        <v>1579</v>
       </c>
       <c r="B449" s="13" t="s">
-        <v>1578</v>
+        <v>1580</v>
       </c>
       <c r="C449" s="13" t="s">
-        <v>1579</v>
+        <v>1581</v>
       </c>
       <c r="D449" s="13" t="s">
-        <v>1580</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="13" t="s">
-        <v>1581</v>
+        <v>1583</v>
       </c>
       <c r="B450" s="13" t="s">
-        <v>1582</v>
+        <v>1584</v>
       </c>
       <c r="C450" s="13" t="s">
-        <v>1583</v>
+        <v>1585</v>
       </c>
       <c r="D450" s="13" t="s">
-        <v>1584</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="13" t="s">
-        <v>1585</v>
+        <v>1587</v>
       </c>
       <c r="B451" s="13" t="s">
-        <v>1586</v>
+        <v>1588</v>
       </c>
       <c r="C451" s="13" t="s">
-        <v>1587</v>
+        <v>1589</v>
       </c>
       <c r="D451" s="13" t="s">
-        <v>1588</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="13" t="s">
-        <v>1589</v>
+        <v>1591</v>
       </c>
       <c r="B452" s="13" t="s">
-        <v>1590</v>
+        <v>1592</v>
       </c>
       <c r="C452" s="13" t="s">
-        <v>1591</v>
+        <v>1593</v>
       </c>
       <c r="D452" s="13" t="s">
-        <v>1592</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="13" t="s">
-        <v>1593</v>
+        <v>1595</v>
       </c>
       <c r="B453" s="13" t="s">
-        <v>1594</v>
+        <v>1596</v>
       </c>
       <c r="C453" s="13" t="s">
-        <v>1595</v>
+        <v>1597</v>
       </c>
       <c r="D453" s="13" t="s">
-        <v>1596</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="13" t="s">
-        <v>1597</v>
+        <v>1599</v>
       </c>
       <c r="B454" s="13" t="s">
-        <v>1598</v>
+        <v>1600</v>
       </c>
       <c r="C454" s="13" t="s">
-        <v>1599</v>
+        <v>1601</v>
       </c>
       <c r="D454" s="13" t="s">
-        <v>1600</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="13" t="s">
-        <v>1601</v>
+        <v>1603</v>
       </c>
       <c r="B455" s="13" t="s">
-        <v>1602</v>
+        <v>1604</v>
       </c>
       <c r="C455" s="13" t="s">
-        <v>1603</v>
+        <v>1605</v>
       </c>
       <c r="D455" s="13" t="s">
-        <v>1604</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="13" t="s">
-        <v>1605</v>
+        <v>1607</v>
       </c>
       <c r="B456" s="13" t="s">
-        <v>1606</v>
+        <v>1608</v>
       </c>
       <c r="C456" s="13" t="s">
-        <v>1607</v>
+        <v>1609</v>
       </c>
       <c r="D456" s="13" t="s">
-        <v>1608</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="13" t="s">
-        <v>1609</v>
+        <v>1611</v>
       </c>
       <c r="B457" s="13" t="s">
-        <v>1610</v>
+        <v>1612</v>
       </c>
       <c r="C457" s="13" t="s">
-        <v>1611</v>
+        <v>1613</v>
       </c>
       <c r="D457" s="13" t="s">
-        <v>1612</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="13" t="s">
-        <v>1613</v>
+        <v>1615</v>
       </c>
       <c r="B458" s="13" t="s">
-        <v>1614</v>
+        <v>1616</v>
       </c>
       <c r="C458" s="13" t="s">
-        <v>1615</v>
+        <v>1617</v>
       </c>
       <c r="D458" s="13" t="s">
-        <v>1616</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="13" t="s">
-        <v>1617</v>
+        <v>1619</v>
       </c>
       <c r="B459" s="13" t="s">
-        <v>1618</v>
+        <v>1620</v>
       </c>
       <c r="C459" s="13" t="s">
-        <v>1619</v>
+        <v>1621</v>
       </c>
       <c r="D459" s="13" t="s">
-        <v>1620</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="13" t="s">
-        <v>1621</v>
+        <v>1623</v>
       </c>
       <c r="B460" s="13" t="s">
-        <v>1622</v>
+        <v>1624</v>
       </c>
       <c r="C460" s="13" t="s">
-        <v>1623</v>
+        <v>1625</v>
       </c>
       <c r="D460" s="13" t="s">
-        <v>1624</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="13" t="s">
-        <v>1625</v>
+        <v>1627</v>
       </c>
       <c r="B461" s="13" t="s">
-        <v>1626</v>
+        <v>1628</v>
       </c>
       <c r="C461" s="13" t="s">
-        <v>1627</v>
+        <v>1629</v>
       </c>
       <c r="D461" s="13" t="s">
-        <v>1628</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="13" t="s">
-        <v>1629</v>
+        <v>1631</v>
       </c>
       <c r="B462" s="13" t="s">
-        <v>1630</v>
+        <v>1632</v>
       </c>
       <c r="C462" s="13" t="s">
-        <v>1631</v>
+        <v>1633</v>
       </c>
       <c r="D462" s="13" t="s">
-        <v>1632</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="13" t="s">
-        <v>1633</v>
+        <v>1635</v>
       </c>
       <c r="B463" s="13" t="s">
-        <v>1634</v>
+        <v>1636</v>
       </c>
       <c r="C463" s="13" t="s">
-        <v>1635</v>
+        <v>1637</v>
       </c>
       <c r="D463" s="13" t="s">
-        <v>1636</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="13" t="s">
-        <v>1637</v>
+        <v>1639</v>
       </c>
       <c r="B464" s="13" t="s">
-        <v>1638</v>
+        <v>1640</v>
       </c>
       <c r="C464" s="13" t="s">
-        <v>1639</v>
+        <v>1641</v>
       </c>
       <c r="D464" s="13" t="s">
-        <v>1640</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="13" t="s">
-        <v>1641</v>
+        <v>1643</v>
       </c>
       <c r="B465" s="13" t="s">
-        <v>1642</v>
+        <v>1644</v>
+      </c>
+      <c r="C465" s="13" t="s">
+        <v>1645</v>
+      </c>
+      <c r="D465" s="13" t="s">
+        <v>1646</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="13" t="s">
-        <v>1643</v>
+        <v>1647</v>
       </c>
       <c r="B466" s="13" t="s">
-        <v>1644</v>
+        <v>1648</v>
       </c>
       <c r="C466" s="13" t="s">
-        <v>1645</v>
+        <v>1649</v>
       </c>
       <c r="D466" s="13" t="s">
-        <v>1646</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="13" t="s">
-        <v>1647</v>
+        <v>1651</v>
       </c>
       <c r="B467" s="13" t="s">
-        <v>1648</v>
+        <v>1652</v>
       </c>
       <c r="C467" s="13" t="s">
-        <v>1649</v>
+        <v>1653</v>
       </c>
       <c r="D467" s="13" t="s">
-        <v>1650</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="13" t="s">
-        <v>1651</v>
+        <v>1655</v>
       </c>
       <c r="B468" s="13" t="s">
-        <v>1652</v>
+        <v>1656</v>
       </c>
       <c r="C468" s="13" t="s">
-        <v>1653</v>
+        <v>1657</v>
       </c>
       <c r="D468" s="13" t="s">
-        <v>1654</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="13" t="s">
-        <v>1655</v>
+        <v>1659</v>
       </c>
       <c r="B469" s="13" t="s">
-        <v>1656</v>
+        <v>1660</v>
       </c>
       <c r="C469" s="13" t="s">
-        <v>1657</v>
+        <v>1661</v>
       </c>
       <c r="D469" s="13" t="s">
-        <v>1658</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="13" t="s">
-        <v>1659</v>
+        <v>1663</v>
       </c>
       <c r="B470" s="13" t="s">
-        <v>1660</v>
+        <v>1664</v>
       </c>
       <c r="C470" s="13" t="s">
-        <v>1661</v>
+        <v>1665</v>
       </c>
       <c r="D470" s="13" t="s">
-        <v>1662</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="13" t="s">
-        <v>1663</v>
+        <v>1667</v>
       </c>
       <c r="B471" s="13" t="s">
-        <v>1664</v>
+        <v>1668</v>
       </c>
       <c r="C471" s="13" t="s">
-        <v>1665</v>
+        <v>1669</v>
       </c>
       <c r="D471" s="13" t="s">
-        <v>1666</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="13" t="s">
-        <v>1667</v>
+        <v>1671</v>
       </c>
       <c r="B472" s="13" t="s">
-        <v>1668</v>
+        <v>1672</v>
       </c>
       <c r="C472" s="13" t="s">
-        <v>1669</v>
+        <v>1673</v>
       </c>
       <c r="D472" s="13" t="s">
-        <v>1670</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="13" t="s">
-        <v>1671</v>
+        <v>1675</v>
       </c>
       <c r="B473" s="13" t="s">
-        <v>1672</v>
+        <v>1676</v>
       </c>
       <c r="C473" s="13" t="s">
-        <v>1673</v>
+        <v>1677</v>
       </c>
       <c r="D473" s="13" t="s">
-        <v>1674</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="13" t="s">
-        <v>1675</v>
+        <v>1679</v>
       </c>
       <c r="B474" s="13" t="s">
-        <v>1676</v>
+        <v>1680</v>
       </c>
       <c r="C474" s="13" t="s">
-        <v>1677</v>
+        <v>1681</v>
       </c>
       <c r="D474" s="13" t="s">
-        <v>1678</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="13" t="s">
-        <v>1679</v>
+        <v>1683</v>
       </c>
       <c r="B475" s="13" t="s">
-        <v>1680</v>
+        <v>1684</v>
       </c>
       <c r="C475" s="13" t="s">
-        <v>1681</v>
+        <v>1685</v>
       </c>
       <c r="D475" s="13" t="s">
-        <v>1682</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="13" t="s">
-        <v>1683</v>
+        <v>1687</v>
       </c>
       <c r="B476" s="13" t="s">
-        <v>1684</v>
+        <v>1688</v>
       </c>
       <c r="C476" s="13" t="s">
-        <v>1685</v>
+        <v>1689</v>
       </c>
       <c r="D476" s="13" t="s">
-        <v>1686</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="13" t="s">
-        <v>1687</v>
+        <v>1691</v>
       </c>
       <c r="B477" s="13" t="s">
-        <v>1688</v>
+        <v>1692</v>
       </c>
       <c r="C477" s="13" t="s">
-        <v>1689</v>
+        <v>1693</v>
       </c>
       <c r="D477" s="13" t="s">
-        <v>1690</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="13" t="s">
-        <v>1691</v>
+        <v>1695</v>
       </c>
       <c r="B478" s="13" t="s">
-        <v>1692</v>
+        <v>1696</v>
       </c>
       <c r="C478" s="13" t="s">
-        <v>1693</v>
+        <v>1697</v>
       </c>
       <c r="D478" s="13" t="s">
-        <v>1694</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="13" t="s">
-        <v>1695</v>
+        <v>1699</v>
       </c>
       <c r="B479" s="13" t="s">
-        <v>1696</v>
+        <v>1700</v>
       </c>
       <c r="C479" s="13" t="s">
-        <v>1697</v>
+        <v>1701</v>
       </c>
       <c r="D479" s="13" t="s">
-        <v>1698</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="13" t="s">
-        <v>1699</v>
+        <v>1703</v>
       </c>
       <c r="B480" s="13" t="s">
-        <v>1700</v>
+        <v>1704</v>
       </c>
       <c r="C480" s="13" t="s">
-        <v>1701</v>
+        <v>1705</v>
       </c>
       <c r="D480" s="13" t="s">
-        <v>1702</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="13" t="s">
-        <v>1703</v>
+        <v>1707</v>
       </c>
       <c r="B481" s="13" t="s">
-        <v>1704</v>
+        <v>1708</v>
       </c>
       <c r="C481" s="13" t="s">
-        <v>1705</v>
+        <v>1709</v>
       </c>
       <c r="D481" s="13" t="s">
-        <v>1706</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="13" t="s">
-        <v>1707</v>
+        <v>1711</v>
       </c>
       <c r="B482" s="13" t="s">
-        <v>1708</v>
+        <v>1712</v>
       </c>
       <c r="C482" s="13" t="s">
-        <v>1709</v>
+        <v>1713</v>
       </c>
       <c r="D482" s="13" t="s">
-        <v>1710</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="13" t="s">
-        <v>1711</v>
+        <v>1715</v>
       </c>
       <c r="B483" s="13" t="s">
-        <v>1712</v>
+        <v>1716</v>
       </c>
       <c r="C483" s="13" t="s">
-        <v>1713</v>
+        <v>1717</v>
       </c>
       <c r="D483" s="13" t="s">
-        <v>1714</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="13" t="s">
-        <v>1715</v>
+        <v>1719</v>
       </c>
       <c r="B484" s="13" t="s">
-        <v>1716</v>
+        <v>1720</v>
       </c>
       <c r="C484" s="13" t="s">
-        <v>1717</v>
+        <v>1721</v>
       </c>
       <c r="D484" s="13" t="s">
-        <v>1718</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="13" t="s">
-        <v>1719</v>
+        <v>1723</v>
       </c>
       <c r="B485" s="13" t="s">
-        <v>1720</v>
+        <v>1724</v>
       </c>
       <c r="C485" s="13" t="s">
-        <v>1721</v>
+        <v>1725</v>
       </c>
       <c r="D485" s="13" t="s">
-        <v>1722</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="13" t="s">
-        <v>1723</v>
+        <v>1727</v>
       </c>
       <c r="B486" s="13" t="s">
-        <v>1724</v>
+        <v>1728</v>
       </c>
       <c r="C486" s="13" t="s">
-        <v>1725</v>
+        <v>1729</v>
       </c>
       <c r="D486" s="13" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A487" s="13" t="s">
-        <v>1727</v>
-      </c>
-      <c r="B487" s="13" t="s">
-        <v>1728</v>
-      </c>
-      <c r="C487" s="13" t="s">
-        <v>1729</v>
-      </c>
-      <c r="D487" s="13" t="s">
         <v>1730</v>
       </c>
     </row>
-    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="488" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="13" t="s">
         <v>1731</v>
       </c>
       <c r="B488" s="13" t="s">
         <v>1732</v>
       </c>
-      <c r="C488" s="13" t="s">
+      <c r="C488" s="15" t="s">
         <v>1733</v>
       </c>
-      <c r="D488" s="13" t="s">
+      <c r="D488" s="15" t="s">
         <v>1734</v>
+      </c>
+    </row>
+    <row r="489" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A489" s="13" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B489" s="13" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C489" s="15" t="s">
+        <v>1737</v>
+      </c>
+      <c r="D489" s="15" t="s">
+        <v>1738</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="13" t="s">
-        <v>1735</v>
+        <v>1739</v>
       </c>
       <c r="B490" s="13" t="s">
-        <v>1736</v>
+        <v>1740</v>
       </c>
       <c r="C490" s="15" t="s">
-        <v>1737</v>
+        <v>1741</v>
       </c>
       <c r="D490" s="15" t="s">
-        <v>1738</v>
-      </c>
-    </row>
-    <row r="491" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="491" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="13" t="s">
-        <v>1739</v>
+        <v>1743</v>
       </c>
       <c r="B491" s="13" t="s">
-        <v>1740</v>
+        <v>1744</v>
       </c>
       <c r="C491" s="15" t="s">
-        <v>1741</v>
+        <v>1745</v>
       </c>
       <c r="D491" s="15" t="s">
-        <v>1742</v>
-      </c>
-    </row>
-    <row r="492" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="492" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="13" t="s">
-        <v>1743</v>
+        <v>1747</v>
       </c>
       <c r="B492" s="13" t="s">
-        <v>1744</v>
+        <v>1748</v>
       </c>
       <c r="C492" s="15" t="s">
-        <v>1745</v>
+        <v>1749</v>
       </c>
       <c r="D492" s="15" t="s">
-        <v>1746</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="13" t="s">
-        <v>1747</v>
+        <v>1751</v>
       </c>
       <c r="B493" s="13" t="s">
-        <v>1748</v>
+        <v>1752</v>
       </c>
       <c r="C493" s="15" t="s">
-        <v>1749</v>
+        <v>1753</v>
       </c>
       <c r="D493" s="15" t="s">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="494" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="494" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="13" t="s">
-        <v>1751</v>
+        <v>1755</v>
       </c>
       <c r="B494" s="13" t="s">
-        <v>1752</v>
+        <v>1756</v>
       </c>
       <c r="C494" s="15" t="s">
-        <v>1753</v>
+        <v>1757</v>
       </c>
       <c r="D494" s="15" t="s">
-        <v>1754</v>
-      </c>
-    </row>
-    <row r="495" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1758</v>
+      </c>
+    </row>
+    <row r="495" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="13" t="s">
-        <v>1755</v>
+        <v>1759</v>
       </c>
       <c r="B495" s="13" t="s">
-        <v>1756</v>
+        <v>1760</v>
       </c>
       <c r="C495" s="15" t="s">
-        <v>1757</v>
+        <v>1761</v>
       </c>
       <c r="D495" s="15" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="496" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="496" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="13" t="s">
-        <v>1759</v>
+        <v>1763</v>
       </c>
       <c r="B496" s="13" t="s">
-        <v>1760</v>
+        <v>1764</v>
       </c>
       <c r="C496" s="15" t="s">
-        <v>1761</v>
+        <v>1765</v>
       </c>
       <c r="D496" s="15" t="s">
-        <v>1762</v>
-      </c>
-    </row>
-    <row r="497" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="16.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A497" s="13" t="s">
-        <v>1763</v>
-      </c>
-      <c r="B497" s="13" t="s">
-        <v>1764</v>
+        <v>1767</v>
+      </c>
+      <c r="B497" s="16" t="s">
+        <v>1768</v>
       </c>
       <c r="C497" s="15" t="s">
-        <v>1765</v>
+        <v>1769</v>
       </c>
       <c r="D497" s="15" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="498" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="13" t="s">
-        <v>1767</v>
+        <v>1771</v>
       </c>
       <c r="B498" s="13" t="s">
-        <v>1768</v>
-      </c>
-      <c r="C498" s="15" t="s">
-        <v>1769</v>
-      </c>
-      <c r="D498" s="15" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="499" customFormat="false" ht="16.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>1772</v>
+      </c>
+      <c r="C498" s="13" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D498" s="13" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="13" t="s">
-        <v>1771</v>
-      </c>
-      <c r="B499" s="17" t="s">
-        <v>1772</v>
-      </c>
-      <c r="C499" s="15" t="s">
-        <v>1773</v>
-      </c>
-      <c r="D499" s="15" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1775</v>
+      </c>
+      <c r="B499" s="13" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C499" s="13" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D499" s="13" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="500" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="13" t="s">
-        <v>1775</v>
+        <v>1779</v>
       </c>
       <c r="B500" s="13" t="s">
-        <v>1776</v>
-      </c>
-      <c r="C500" s="13" t="s">
-        <v>1777</v>
-      </c>
-      <c r="D500" s="13" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1780</v>
+      </c>
+      <c r="C500" s="15" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D500" s="15" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="501" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="13" t="s">
-        <v>1779</v>
+        <v>1781</v>
       </c>
       <c r="B501" s="13" t="s">
-        <v>1780</v>
-      </c>
-      <c r="C501" s="13" t="s">
-        <v>1781</v>
-      </c>
-      <c r="D501" s="13" t="s">
         <v>1782</v>
+      </c>
+      <c r="C501" s="15" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D501" s="15" t="s">
+        <v>1375</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39195,70 +39189,42 @@
         <v>1784</v>
       </c>
       <c r="C502" s="15" t="s">
-        <v>1372</v>
+        <v>1378</v>
       </c>
       <c r="D502" s="15" t="s">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="503" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A503" s="13" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A503" s="17" t="s">
         <v>1785</v>
       </c>
       <c r="B503" s="13" t="s">
         <v>1786</v>
       </c>
-      <c r="C503" s="15" t="s">
-        <v>1376</v>
-      </c>
-      <c r="D503" s="15" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="504" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C503" s="13" t="s">
+        <v>1787</v>
+      </c>
+      <c r="D503" s="13" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="13" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="B504" s="13" t="s">
-        <v>1788</v>
-      </c>
-      <c r="C504" s="15" t="s">
-        <v>1380</v>
-      </c>
-      <c r="D504" s="15" t="s">
-        <v>1381</v>
-      </c>
-    </row>
-    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="18" t="s">
         <v>1789</v>
       </c>
-      <c r="B505" s="13" t="s">
+      <c r="C504" s="13" t="s">
         <v>1790</v>
       </c>
-      <c r="C505" s="13" t="s">
+      <c r="D504" s="13" t="s">
         <v>1791</v>
       </c>
-      <c r="D505" s="13" t="s">
-        <v>1791</v>
-      </c>
-    </row>
-    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A506" s="13" t="s">
-        <v>1792</v>
-      </c>
-      <c r="B506" s="13" t="s">
-        <v>1793</v>
-      </c>
-      <c r="C506" s="13" t="s">
-        <v>1794</v>
-      </c>
-      <c r="D506" s="13" t="s">
-        <v>1795</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:D1 B398:D406 B410:D410 B413:D439 B506:B1048576 C69:D357 C370:D370 C395:D489 D506:D1048576 C500:D501 C372:D375 C506:C1048576 C364:D367 C384:D384 C1:D64 C392:C393 B500:B504 C503:C504 B505:D505 B1:B498">
+  <conditionalFormatting sqref="B1:D1 B397:D405 B409:D409 B412:D438 B504:B1048576 C69:D357 C369:D369 C464:D487 D504:D1048576 C498:D499 C371:D374 C504:C1048576 C363:D366 C383:D383 C1:D64 C391:C392 B498:B502 C501:C502 B503:D503 B1:B496 C394:D463">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update translations for forms
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3431" uniqueCount="1781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3467" uniqueCount="1795">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -3282,6 +3282,12 @@
     <t xml:space="preserve"> 31</t>
   </si>
   <si>
+    <t xml:space="preserve">Agusti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disemba</t>
+  </si>
+  <si>
     <t xml:space="preserve"> 2021</t>
   </si>
   <si>
@@ -4137,30 +4143,60 @@
     <t xml:space="preserve">Invalid date month combination</t>
   </si>
   <si>
+    <t xml:space="preserve">Combinação de data / mês inválida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarehe na Mwezi si sahihi</t>
+  </si>
+  <si>
     <t xml:space="preserve">invalid_dmy</t>
   </si>
   <si>
     <t xml:space="preserve">Invalid date month year combination</t>
   </si>
   <si>
+    <t xml:space="preserve">Combinação inválida de data, mês e ano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarehe,Mwezi na Mwaka si sahihi</t>
+  </si>
+  <si>
     <t xml:space="preserve">invalid_time_q31</t>
   </si>
   <si>
     <t xml:space="preserve">The answer to Q31 cannot be earlier than that of Q30</t>
   </si>
   <si>
+    <t xml:space="preserve">A resposta a Q31 não pode ser anterior a Q30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jibu la swali la Q31 haliwezi kuwa kabla ya jibu la Q30</t>
+  </si>
+  <si>
     <t xml:space="preserve">invalid_time_q28</t>
   </si>
   <si>
     <t xml:space="preserve">The answer to Q28 cannot be earlier than that of Q27</t>
   </si>
   <si>
+    <t xml:space="preserve">A resposta à Q28 não pode ser anterior à Q27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jibu la swali la Q28 haliwezi kuwa kabla ya jibu la Q27</t>
+  </si>
+  <si>
     <t xml:space="preserve">unexpected_trips</t>
   </si>
   <si>
     <t xml:space="preserve">Unexpected number of trips recorded</t>
   </si>
   <si>
+    <t xml:space="preserve">Número inesperado de viagens registradas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idadi isiyotarajiwa ya safari zilizorekodiwa</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Given name:</t>
   </si>
   <si>
@@ -5356,6 +5392,12 @@
   </si>
   <si>
     <t xml:space="preserve">The household head should be the first member added and must be a resident member. His/her ExtID should end in -001 unless he/she has an existing ID assigned from the minicensus. The substitue household head, if there is one, must also be a resident member.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O chefe do agregado deve ser o primeiro membro adicionado e deve ser um membro residente. Seu ExtID deve terminar em - 001, a menos que ele / ela tenha um ID existente atribuído a partir do minicenso. O chefe substituto do agregado , se houver, também deve ser residente.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mkuu wa kaya lazima awe wa kwanza kauandikishwa na lazima awe mkazi. Namba yake ya utambulisho inatakiwa kuishia na 001vinginevyo awe na namba ya utambulisho kutoka aliyopewa kwenye sensafupi (minicensus). Mbadala wa mkuu wa kaya, endapo yupo, ni lazima awe mkazi.</t>
   </si>
   <si>
     <t xml:space="preserve">check_all_that_apply_hint</t>
@@ -5746,7 +5788,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.69"/>
   </cols>
@@ -6797,11 +6839,10 @@
       <selection pane="topLeft" activeCell="N30" activeCellId="0" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.28"/>
@@ -8307,7 +8348,7 @@
       <selection pane="bottomLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.16"/>
@@ -13580,7 +13621,7 @@
       <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.53125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.79"/>
@@ -31212,7 +31253,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.04"/>
@@ -32356,9 +32397,9 @@
   <dimension ref="A1:D502"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A487" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A154" activeCellId="0" sqref="A154"/>
+      <selection pane="bottomLeft" activeCell="C501" activeCellId="0" sqref="C501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35441,6 +35482,12 @@
       <c r="B221" s="14" t="s">
         <v>857</v>
       </c>
+      <c r="C221" s="14" t="s">
+        <v>858</v>
+      </c>
+      <c r="D221" s="14" t="s">
+        <v>859</v>
+      </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="14" t="s">
@@ -35449,6 +35496,12 @@
       <c r="B222" s="14" t="s">
         <v>860</v>
       </c>
+      <c r="C222" s="14" t="s">
+        <v>861</v>
+      </c>
+      <c r="D222" s="14" t="s">
+        <v>862</v>
+      </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="14" t="s">
@@ -35457,6 +35510,12 @@
       <c r="B223" s="14" t="s">
         <v>863</v>
       </c>
+      <c r="C223" s="14" t="s">
+        <v>864</v>
+      </c>
+      <c r="D223" s="14" t="s">
+        <v>865</v>
+      </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="14" t="s">
@@ -35465,6 +35524,12 @@
       <c r="B224" s="14" t="s">
         <v>866</v>
       </c>
+      <c r="C224" s="14" t="s">
+        <v>867</v>
+      </c>
+      <c r="D224" s="14" t="s">
+        <v>868</v>
+      </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="14" t="s">
@@ -35473,6 +35538,12 @@
       <c r="B225" s="14" t="s">
         <v>869</v>
       </c>
+      <c r="C225" s="14" t="s">
+        <v>870</v>
+      </c>
+      <c r="D225" s="14" t="s">
+        <v>871</v>
+      </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="14" t="s">
@@ -35481,6 +35552,12 @@
       <c r="B226" s="14" t="s">
         <v>872</v>
       </c>
+      <c r="C226" s="14" t="s">
+        <v>873</v>
+      </c>
+      <c r="D226" s="14" t="s">
+        <v>874</v>
+      </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="14" t="s">
@@ -35489,6 +35566,12 @@
       <c r="B227" s="14" t="s">
         <v>875</v>
       </c>
+      <c r="C227" s="14" t="s">
+        <v>876</v>
+      </c>
+      <c r="D227" s="14" t="s">
+        <v>877</v>
+      </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="14" t="s">
@@ -35497,6 +35580,12 @@
       <c r="B228" s="14" t="s">
         <v>878</v>
       </c>
+      <c r="C228" s="14" t="s">
+        <v>879</v>
+      </c>
+      <c r="D228" s="14" t="s">
+        <v>1085</v>
+      </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="14" t="s">
@@ -35505,6 +35594,12 @@
       <c r="B229" s="14" t="s">
         <v>881</v>
       </c>
+      <c r="C229" s="14" t="s">
+        <v>882</v>
+      </c>
+      <c r="D229" s="14" t="s">
+        <v>883</v>
+      </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="14" t="s">
@@ -35513,6 +35608,12 @@
       <c r="B230" s="14" t="s">
         <v>884</v>
       </c>
+      <c r="C230" s="14" t="s">
+        <v>885</v>
+      </c>
+      <c r="D230" s="14" t="s">
+        <v>886</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="14" t="s">
@@ -35521,6 +35622,12 @@
       <c r="B231" s="14" t="s">
         <v>887</v>
       </c>
+      <c r="C231" s="14" t="s">
+        <v>888</v>
+      </c>
+      <c r="D231" s="14" t="s">
+        <v>889</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="14" t="s">
@@ -35529,19 +35636,25 @@
       <c r="B232" s="14" t="s">
         <v>890</v>
       </c>
+      <c r="C232" s="14" t="s">
+        <v>891</v>
+      </c>
+      <c r="D232" s="14" t="s">
+        <v>1086</v>
+      </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="14" t="s">
         <v>351</v>
       </c>
       <c r="B233" s="14" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="C233" s="14" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="D233" s="14" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35549,13 +35662,13 @@
         <v>352</v>
       </c>
       <c r="B234" s="14" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="C234" s="14" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="D234" s="14" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35563,13 +35676,13 @@
         <v>353</v>
       </c>
       <c r="B235" s="14" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="C235" s="14" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="D235" s="14" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35577,13 +35690,13 @@
         <v>354</v>
       </c>
       <c r="B236" s="14" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="C236" s="14" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="D236" s="14" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35591,13 +35704,13 @@
         <v>355</v>
       </c>
       <c r="B237" s="14" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="C237" s="14" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="D237" s="14" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35605,13 +35718,13 @@
         <v>356</v>
       </c>
       <c r="B238" s="14" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="C238" s="14" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="D238" s="14" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35619,13 +35732,13 @@
         <v>357</v>
       </c>
       <c r="B239" s="14" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="C239" s="14" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="D239" s="14" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35633,13 +35746,13 @@
         <v>358</v>
       </c>
       <c r="B240" s="14" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="C240" s="14" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="D240" s="14" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35647,13 +35760,13 @@
         <v>359</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="C241" s="14" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="D241" s="14" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35661,13 +35774,13 @@
         <v>360</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="D242" s="14" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35675,13 +35788,13 @@
         <v>361</v>
       </c>
       <c r="B243" s="14" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="C243" s="14" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="D243" s="14" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35689,13 +35802,13 @@
         <v>362</v>
       </c>
       <c r="B244" s="14" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="C244" s="14" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="D244" s="14" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35703,13 +35816,13 @@
         <v>363</v>
       </c>
       <c r="B245" s="14" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="C245" s="14" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="D245" s="14" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35717,13 +35830,13 @@
         <v>364</v>
       </c>
       <c r="B246" s="14" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="C246" s="14" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="D246" s="14" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35731,13 +35844,13 @@
         <v>365</v>
       </c>
       <c r="B247" s="14" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="C247" s="14" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="D247" s="14" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35745,13 +35858,13 @@
         <v>366</v>
       </c>
       <c r="B248" s="14" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="C248" s="14" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="D248" s="14" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35759,13 +35872,13 @@
         <v>367</v>
       </c>
       <c r="B249" s="14" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="C249" s="14" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="D249" s="14" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35773,13 +35886,13 @@
         <v>368</v>
       </c>
       <c r="B250" s="14" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="C250" s="14" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="D250" s="14" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35787,13 +35900,13 @@
         <v>369</v>
       </c>
       <c r="B251" s="14" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="C251" s="14" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="D251" s="14" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35801,13 +35914,13 @@
         <v>370</v>
       </c>
       <c r="B252" s="14" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="C252" s="14" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="D252" s="14" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35815,13 +35928,13 @@
         <v>371</v>
       </c>
       <c r="B253" s="14" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
       <c r="C253" s="14" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
       <c r="D253" s="14" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35829,13 +35942,13 @@
         <v>372</v>
       </c>
       <c r="B254" s="14" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="C254" s="14" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="D254" s="14" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35843,13 +35956,13 @@
         <v>373</v>
       </c>
       <c r="B255" s="14" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="C255" s="14" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="D255" s="14" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35857,13 +35970,13 @@
         <v>374</v>
       </c>
       <c r="B256" s="14" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="C256" s="14" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="D256" s="14" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35871,13 +35984,13 @@
         <v>375</v>
       </c>
       <c r="B257" s="14" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="C257" s="14" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="D257" s="14" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35885,13 +35998,13 @@
         <v>376</v>
       </c>
       <c r="B258" s="14" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="C258" s="14" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="D258" s="14" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35899,13 +36012,13 @@
         <v>377</v>
       </c>
       <c r="B259" s="14" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="C259" s="14" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="D259" s="14" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35913,13 +36026,13 @@
         <v>378</v>
       </c>
       <c r="B260" s="14" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="C260" s="14" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D260" s="14" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35927,13 +36040,13 @@
         <v>379</v>
       </c>
       <c r="B261" s="14" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="C261" s="14" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="D261" s="14" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35941,13 +36054,13 @@
         <v>380</v>
       </c>
       <c r="B262" s="14" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="C262" s="14" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="D262" s="14" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35955,13 +36068,13 @@
         <v>381</v>
       </c>
       <c r="B263" s="14" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="C263" s="14" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="D263" s="14" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35969,13 +36082,13 @@
         <v>382</v>
       </c>
       <c r="B264" s="14" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="C264" s="14" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="D264" s="14" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35983,13 +36096,13 @@
         <v>383</v>
       </c>
       <c r="B265" s="14" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="C265" s="14" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="D265" s="14" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35997,13 +36110,13 @@
         <v>384</v>
       </c>
       <c r="B266" s="14" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="C266" s="14" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="D266" s="14" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36011,13 +36124,13 @@
         <v>385</v>
       </c>
       <c r="B267" s="14" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="C267" s="14" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="D267" s="14" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36025,13 +36138,13 @@
         <v>386</v>
       </c>
       <c r="B268" s="14" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="C268" s="14" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="D268" s="14" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36039,13 +36152,13 @@
         <v>387</v>
       </c>
       <c r="B269" s="14" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="C269" s="14" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="D269" s="14" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36053,13 +36166,13 @@
         <v>388</v>
       </c>
       <c r="B270" s="14" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="C270" s="14" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="D270" s="14" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36067,13 +36180,13 @@
         <v>389</v>
       </c>
       <c r="B271" s="14" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="C271" s="14" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="D271" s="14" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36081,13 +36194,13 @@
         <v>390</v>
       </c>
       <c r="B272" s="14" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="C272" s="14" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="D272" s="14" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36095,13 +36208,13 @@
         <v>391</v>
       </c>
       <c r="B273" s="14" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="C273" s="14" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="D273" s="14" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36109,13 +36222,13 @@
         <v>392</v>
       </c>
       <c r="B274" s="14" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="C274" s="14" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="D274" s="14" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36123,13 +36236,13 @@
         <v>393</v>
       </c>
       <c r="B275" s="14" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="C275" s="14" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="D275" s="14" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36137,13 +36250,13 @@
         <v>394</v>
       </c>
       <c r="B276" s="14" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="C276" s="14" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="D276" s="14" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36151,13 +36264,13 @@
         <v>395</v>
       </c>
       <c r="B277" s="14" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="C277" s="14" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="D277" s="14" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36165,13 +36278,13 @@
         <v>396</v>
       </c>
       <c r="B278" s="14" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="C278" s="14" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="D278" s="14" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36179,13 +36292,13 @@
         <v>397</v>
       </c>
       <c r="B279" s="14" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="C279" s="14" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="D279" s="14" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36193,13 +36306,13 @@
         <v>398</v>
       </c>
       <c r="B280" s="14" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
       <c r="C280" s="14" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
       <c r="D280" s="14" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36207,13 +36320,13 @@
         <v>399</v>
       </c>
       <c r="B281" s="14" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="C281" s="14" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="D281" s="14" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36221,13 +36334,13 @@
         <v>400</v>
       </c>
       <c r="B282" s="14" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="C282" s="14" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="D282" s="14" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36235,13 +36348,13 @@
         <v>401</v>
       </c>
       <c r="B283" s="14" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="C283" s="14" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="D283" s="14" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36249,13 +36362,13 @@
         <v>402</v>
       </c>
       <c r="B284" s="14" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="C284" s="14" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="D284" s="14" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36263,13 +36376,13 @@
         <v>403</v>
       </c>
       <c r="B285" s="14" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="C285" s="14" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="D285" s="14" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36277,13 +36390,13 @@
         <v>404</v>
       </c>
       <c r="B286" s="14" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="C286" s="14" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="D286" s="14" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36291,13 +36404,13 @@
         <v>405</v>
       </c>
       <c r="B287" s="14" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="C287" s="14" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="D287" s="14" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36305,13 +36418,13 @@
         <v>406</v>
       </c>
       <c r="B288" s="14" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="C288" s="14" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="D288" s="14" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36319,13 +36432,13 @@
         <v>407</v>
       </c>
       <c r="B289" s="14" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="C289" s="14" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="D289" s="14" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36333,13 +36446,13 @@
         <v>408</v>
       </c>
       <c r="B290" s="14" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="C290" s="14" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="D290" s="14" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36347,13 +36460,13 @@
         <v>409</v>
       </c>
       <c r="B291" s="14" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="C291" s="14" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="D291" s="14" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36361,13 +36474,13 @@
         <v>410</v>
       </c>
       <c r="B292" s="14" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="C292" s="14" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="D292" s="14" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36375,13 +36488,13 @@
         <v>411</v>
       </c>
       <c r="B293" s="14" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="C293" s="14" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="D293" s="14" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36389,13 +36502,13 @@
         <v>412</v>
       </c>
       <c r="B294" s="14" t="s">
-        <v>1146</v>
+        <v>1148</v>
       </c>
       <c r="C294" s="14" t="s">
-        <v>1146</v>
+        <v>1148</v>
       </c>
       <c r="D294" s="14" t="s">
-        <v>1146</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36403,13 +36516,13 @@
         <v>413</v>
       </c>
       <c r="B295" s="14" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="C295" s="14" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="D295" s="14" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36417,13 +36530,13 @@
         <v>414</v>
       </c>
       <c r="B296" s="14" t="s">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="C296" s="14" t="s">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="D296" s="14" t="s">
-        <v>1148</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36431,13 +36544,13 @@
         <v>415</v>
       </c>
       <c r="B297" s="14" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
       <c r="C297" s="14" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
       <c r="D297" s="14" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36445,13 +36558,13 @@
         <v>416</v>
       </c>
       <c r="B298" s="14" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="C298" s="14" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="D298" s="14" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36459,13 +36572,13 @@
         <v>417</v>
       </c>
       <c r="B299" s="14" t="s">
-        <v>1151</v>
+        <v>1153</v>
       </c>
       <c r="C299" s="14" t="s">
-        <v>1151</v>
+        <v>1153</v>
       </c>
       <c r="D299" s="14" t="s">
-        <v>1151</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36473,13 +36586,13 @@
         <v>418</v>
       </c>
       <c r="B300" s="14" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="C300" s="14" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="D300" s="14" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36487,13 +36600,13 @@
         <v>419</v>
       </c>
       <c r="B301" s="14" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="C301" s="14" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="D301" s="14" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36501,13 +36614,13 @@
         <v>420</v>
       </c>
       <c r="B302" s="14" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="C302" s="14" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="D302" s="14" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36515,13 +36628,13 @@
         <v>421</v>
       </c>
       <c r="B303" s="14" t="s">
-        <v>1155</v>
+        <v>1157</v>
       </c>
       <c r="C303" s="14" t="s">
-        <v>1155</v>
+        <v>1157</v>
       </c>
       <c r="D303" s="14" t="s">
-        <v>1155</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36529,13 +36642,13 @@
         <v>422</v>
       </c>
       <c r="B304" s="14" t="s">
-        <v>1156</v>
+        <v>1158</v>
       </c>
       <c r="C304" s="14" t="s">
-        <v>1156</v>
+        <v>1158</v>
       </c>
       <c r="D304" s="14" t="s">
-        <v>1156</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36543,13 +36656,13 @@
         <v>423</v>
       </c>
       <c r="B305" s="14" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="C305" s="14" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="D305" s="14" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36557,13 +36670,13 @@
         <v>424</v>
       </c>
       <c r="B306" s="14" t="s">
-        <v>1158</v>
+        <v>1160</v>
       </c>
       <c r="C306" s="14" t="s">
-        <v>1158</v>
+        <v>1160</v>
       </c>
       <c r="D306" s="14" t="s">
-        <v>1158</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36571,13 +36684,13 @@
         <v>425</v>
       </c>
       <c r="B307" s="14" t="s">
-        <v>1159</v>
+        <v>1161</v>
       </c>
       <c r="C307" s="14" t="s">
-        <v>1159</v>
+        <v>1161</v>
       </c>
       <c r="D307" s="14" t="s">
-        <v>1159</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36585,13 +36698,13 @@
         <v>426</v>
       </c>
       <c r="B308" s="14" t="s">
-        <v>1160</v>
+        <v>1162</v>
       </c>
       <c r="C308" s="14" t="s">
-        <v>1160</v>
+        <v>1162</v>
       </c>
       <c r="D308" s="14" t="s">
-        <v>1160</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36599,13 +36712,13 @@
         <v>427</v>
       </c>
       <c r="B309" s="14" t="s">
-        <v>1161</v>
+        <v>1163</v>
       </c>
       <c r="C309" s="14" t="s">
-        <v>1161</v>
+        <v>1163</v>
       </c>
       <c r="D309" s="14" t="s">
-        <v>1161</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36613,13 +36726,13 @@
         <v>428</v>
       </c>
       <c r="B310" s="14" t="s">
-        <v>1162</v>
+        <v>1164</v>
       </c>
       <c r="C310" s="14" t="s">
-        <v>1162</v>
+        <v>1164</v>
       </c>
       <c r="D310" s="14" t="s">
-        <v>1162</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36627,13 +36740,13 @@
         <v>429</v>
       </c>
       <c r="B311" s="14" t="s">
-        <v>1163</v>
+        <v>1165</v>
       </c>
       <c r="C311" s="14" t="s">
-        <v>1163</v>
+        <v>1165</v>
       </c>
       <c r="D311" s="14" t="s">
-        <v>1163</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36641,13 +36754,13 @@
         <v>430</v>
       </c>
       <c r="B312" s="14" t="s">
-        <v>1164</v>
+        <v>1166</v>
       </c>
       <c r="C312" s="14" t="s">
-        <v>1164</v>
+        <v>1166</v>
       </c>
       <c r="D312" s="14" t="s">
-        <v>1164</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36655,13 +36768,13 @@
         <v>431</v>
       </c>
       <c r="B313" s="14" t="s">
-        <v>1165</v>
+        <v>1167</v>
       </c>
       <c r="C313" s="14" t="s">
-        <v>1165</v>
+        <v>1167</v>
       </c>
       <c r="D313" s="14" t="s">
-        <v>1165</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36669,13 +36782,13 @@
         <v>432</v>
       </c>
       <c r="B314" s="14" t="s">
-        <v>1166</v>
+        <v>1168</v>
       </c>
       <c r="C314" s="14" t="s">
-        <v>1166</v>
+        <v>1168</v>
       </c>
       <c r="D314" s="14" t="s">
-        <v>1166</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36683,13 +36796,13 @@
         <v>433</v>
       </c>
       <c r="B315" s="14" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
       <c r="C315" s="14" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
       <c r="D315" s="14" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36697,13 +36810,13 @@
         <v>434</v>
       </c>
       <c r="B316" s="14" t="s">
-        <v>1168</v>
+        <v>1170</v>
       </c>
       <c r="C316" s="14" t="s">
-        <v>1168</v>
+        <v>1170</v>
       </c>
       <c r="D316" s="14" t="s">
-        <v>1168</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36711,13 +36824,13 @@
         <v>435</v>
       </c>
       <c r="B317" s="14" t="s">
-        <v>1169</v>
+        <v>1171</v>
       </c>
       <c r="C317" s="14" t="s">
-        <v>1169</v>
+        <v>1171</v>
       </c>
       <c r="D317" s="14" t="s">
-        <v>1169</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36725,13 +36838,13 @@
         <v>436</v>
       </c>
       <c r="B318" s="14" t="s">
-        <v>1170</v>
+        <v>1172</v>
       </c>
       <c r="C318" s="14" t="s">
-        <v>1170</v>
+        <v>1172</v>
       </c>
       <c r="D318" s="14" t="s">
-        <v>1170</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36739,13 +36852,13 @@
         <v>437</v>
       </c>
       <c r="B319" s="14" t="s">
-        <v>1171</v>
+        <v>1173</v>
       </c>
       <c r="C319" s="14" t="s">
-        <v>1171</v>
+        <v>1173</v>
       </c>
       <c r="D319" s="14" t="s">
-        <v>1171</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36753,13 +36866,13 @@
         <v>438</v>
       </c>
       <c r="B320" s="14" t="s">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="C320" s="14" t="s">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="D320" s="14" t="s">
-        <v>1172</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36767,13 +36880,13 @@
         <v>439</v>
       </c>
       <c r="B321" s="14" t="s">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="C321" s="14" t="s">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="D321" s="14" t="s">
-        <v>1173</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36781,13 +36894,13 @@
         <v>440</v>
       </c>
       <c r="B322" s="14" t="s">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c r="C322" s="14" t="s">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c r="D322" s="14" t="s">
-        <v>1174</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36795,13 +36908,13 @@
         <v>441</v>
       </c>
       <c r="B323" s="14" t="s">
-        <v>1175</v>
+        <v>1177</v>
       </c>
       <c r="C323" s="14" t="s">
-        <v>1175</v>
+        <v>1177</v>
       </c>
       <c r="D323" s="14" t="s">
-        <v>1175</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36809,13 +36922,13 @@
         <v>442</v>
       </c>
       <c r="B324" s="14" t="s">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="C324" s="14" t="s">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="D324" s="14" t="s">
-        <v>1176</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36823,13 +36936,13 @@
         <v>443</v>
       </c>
       <c r="B325" s="14" t="s">
-        <v>1177</v>
+        <v>1179</v>
       </c>
       <c r="C325" s="14" t="s">
-        <v>1177</v>
+        <v>1179</v>
       </c>
       <c r="D325" s="14" t="s">
-        <v>1177</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36837,13 +36950,13 @@
         <v>444</v>
       </c>
       <c r="B326" s="14" t="s">
-        <v>1178</v>
+        <v>1180</v>
       </c>
       <c r="C326" s="14" t="s">
-        <v>1178</v>
+        <v>1180</v>
       </c>
       <c r="D326" s="14" t="s">
-        <v>1178</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36851,13 +36964,13 @@
         <v>445</v>
       </c>
       <c r="B327" s="14" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="C327" s="14" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="D327" s="14" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36865,13 +36978,13 @@
         <v>446</v>
       </c>
       <c r="B328" s="14" t="s">
-        <v>1180</v>
+        <v>1182</v>
       </c>
       <c r="C328" s="14" t="s">
-        <v>1180</v>
+        <v>1182</v>
       </c>
       <c r="D328" s="14" t="s">
-        <v>1180</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36879,13 +36992,13 @@
         <v>447</v>
       </c>
       <c r="B329" s="14" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="C329" s="14" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="D329" s="14" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36893,13 +37006,13 @@
         <v>448</v>
       </c>
       <c r="B330" s="14" t="s">
-        <v>1182</v>
+        <v>1184</v>
       </c>
       <c r="C330" s="14" t="s">
-        <v>1182</v>
+        <v>1184</v>
       </c>
       <c r="D330" s="14" t="s">
-        <v>1182</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36907,13 +37020,13 @@
         <v>449</v>
       </c>
       <c r="B331" s="14" t="s">
-        <v>1183</v>
+        <v>1185</v>
       </c>
       <c r="C331" s="14" t="s">
-        <v>1183</v>
+        <v>1185</v>
       </c>
       <c r="D331" s="14" t="s">
-        <v>1183</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36921,13 +37034,13 @@
         <v>450</v>
       </c>
       <c r="B332" s="14" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="C332" s="14" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="D332" s="14" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36935,13 +37048,13 @@
         <v>451</v>
       </c>
       <c r="B333" s="14" t="s">
-        <v>1185</v>
+        <v>1187</v>
       </c>
       <c r="C333" s="14" t="s">
-        <v>1185</v>
+        <v>1187</v>
       </c>
       <c r="D333" s="14" t="s">
-        <v>1185</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -36949,181 +37062,181 @@
         <v>452</v>
       </c>
       <c r="B334" s="14" t="s">
-        <v>1186</v>
+        <v>1188</v>
       </c>
       <c r="C334" s="14" t="s">
-        <v>1186</v>
+        <v>1188</v>
       </c>
       <c r="D334" s="14" t="s">
-        <v>1186</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="14" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="B336" s="14" t="s">
-        <v>1188</v>
+        <v>1190</v>
       </c>
       <c r="C336" s="14" t="s">
-        <v>1189</v>
+        <v>1191</v>
       </c>
       <c r="D336" s="14" t="s">
-        <v>1190</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="14" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="B337" s="14" t="s">
-        <v>1192</v>
+        <v>1194</v>
       </c>
       <c r="C337" s="14" t="s">
-        <v>1193</v>
+        <v>1195</v>
       </c>
       <c r="D337" s="14" t="s">
-        <v>1194</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="14" t="s">
-        <v>1195</v>
+        <v>1197</v>
       </c>
       <c r="B338" s="14" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
       <c r="C338" s="14" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="D338" s="14" t="s">
-        <v>1198</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="14" t="s">
-        <v>1199</v>
+        <v>1201</v>
       </c>
       <c r="B339" s="14" t="s">
-        <v>1200</v>
+        <v>1202</v>
       </c>
       <c r="C339" s="14" t="s">
-        <v>1201</v>
+        <v>1203</v>
       </c>
       <c r="D339" s="14" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="14" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
       <c r="B340" s="14" t="s">
-        <v>1204</v>
+        <v>1206</v>
       </c>
       <c r="C340" s="14" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
       <c r="D340" s="14" t="s">
-        <v>1206</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="14" t="s">
-        <v>1207</v>
+        <v>1209</v>
       </c>
       <c r="B342" s="14" t="s">
-        <v>1208</v>
+        <v>1210</v>
       </c>
       <c r="C342" s="14" t="s">
-        <v>1209</v>
+        <v>1211</v>
       </c>
       <c r="D342" s="14" t="s">
-        <v>1210</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="14" t="s">
-        <v>1211</v>
+        <v>1213</v>
       </c>
       <c r="B343" s="14" t="s">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="C343" s="14" t="s">
-        <v>1213</v>
+        <v>1215</v>
       </c>
       <c r="D343" s="14" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="14" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="B344" s="14" t="s">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="C344" s="14" t="s">
-        <v>1217</v>
+        <v>1219</v>
       </c>
       <c r="D344" s="14" t="s">
-        <v>1218</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="14" t="s">
-        <v>1219</v>
+        <v>1221</v>
       </c>
       <c r="B345" s="14" t="s">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="C345" s="14" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="D345" s="14" t="s">
-        <v>1222</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="14" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
       <c r="B346" s="14" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="C346" s="14" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="D346" s="14" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="14" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="B347" s="14" t="s">
-        <v>1228</v>
+        <v>1230</v>
       </c>
       <c r="C347" s="14" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="D347" s="14" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="14" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="B348" s="14" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="C348" s="14" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
       <c r="D348" s="14" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37131,7 +37244,7 @@
         <v>34</v>
       </c>
       <c r="B350" s="14" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="C350" s="14" t="s">
         <v>743</v>
@@ -37145,7 +37258,7 @@
         <v>46</v>
       </c>
       <c r="B351" s="14" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="C351" s="14" t="s">
         <v>749</v>
@@ -37159,7 +37272,7 @@
         <v>52</v>
       </c>
       <c r="B352" s="14" t="s">
-        <v>1237</v>
+        <v>1239</v>
       </c>
       <c r="C352" s="14" t="s">
         <v>757</v>
@@ -37173,27 +37286,27 @@
         <v>74</v>
       </c>
       <c r="B353" s="14" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
       <c r="C353" s="14" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
       <c r="D353" s="14" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="14" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
       <c r="B354" s="14" t="s">
-        <v>1242</v>
+        <v>1244</v>
       </c>
       <c r="C354" s="14" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="D354" s="14" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37201,181 +37314,181 @@
         <v>155</v>
       </c>
       <c r="B355" s="14" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
       <c r="C355" s="14" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="D355" s="14" t="s">
-        <v>1247</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="14" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
       <c r="B356" s="14" t="s">
-        <v>1249</v>
+        <v>1251</v>
       </c>
       <c r="C356" s="14" t="s">
-        <v>1250</v>
+        <v>1252</v>
       </c>
       <c r="D356" s="14" t="s">
-        <v>1251</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="14" t="s">
-        <v>1252</v>
+        <v>1254</v>
       </c>
       <c r="B357" s="14" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="C357" s="14" t="s">
-        <v>1254</v>
+        <v>1256</v>
       </c>
       <c r="D357" s="14" t="s">
-        <v>1255</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="14" t="s">
-        <v>1256</v>
+        <v>1258</v>
       </c>
       <c r="B358" s="14" t="s">
-        <v>1257</v>
+        <v>1259</v>
       </c>
       <c r="C358" s="14" t="s">
-        <v>1258</v>
+        <v>1260</v>
       </c>
       <c r="D358" s="14" t="s">
-        <v>1259</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="14" t="s">
-        <v>1260</v>
+        <v>1262</v>
       </c>
       <c r="B359" s="14" t="s">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="C359" s="16" t="s">
-        <v>1262</v>
+        <v>1264</v>
       </c>
       <c r="D359" s="16" t="s">
-        <v>1263</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="14" t="s">
-        <v>1264</v>
+        <v>1266</v>
       </c>
       <c r="B360" s="14" t="s">
-        <v>1265</v>
+        <v>1267</v>
       </c>
       <c r="C360" s="16" t="s">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="D360" s="16" t="s">
-        <v>1267</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="14" t="s">
-        <v>1268</v>
+        <v>1270</v>
       </c>
       <c r="B361" s="14" t="s">
-        <v>1269</v>
+        <v>1271</v>
       </c>
       <c r="C361" s="14" t="s">
-        <v>1270</v>
+        <v>1272</v>
       </c>
       <c r="D361" s="14" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="14" t="s">
-        <v>1272</v>
+        <v>1274</v>
       </c>
       <c r="B362" s="14" t="s">
-        <v>1273</v>
+        <v>1275</v>
       </c>
       <c r="C362" s="16" t="s">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="D362" s="16" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="14" t="s">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="B363" s="14" t="s">
-        <v>1277</v>
+        <v>1279</v>
       </c>
       <c r="C363" s="14" t="s">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="D363" s="14" t="s">
-        <v>1279</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="14" t="s">
-        <v>1280</v>
+        <v>1282</v>
       </c>
       <c r="B364" s="14" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="C364" s="14" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="D364" s="14" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="14" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="B365" s="14" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="C365" s="16" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="D365" s="16" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="14" t="s">
-        <v>1286</v>
+        <v>1288</v>
       </c>
       <c r="B366" s="14" t="s">
-        <v>1287</v>
+        <v>1289</v>
       </c>
       <c r="C366" s="14" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
       <c r="D366" s="14" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="14" t="s">
-        <v>1290</v>
+        <v>1292</v>
       </c>
       <c r="B367" s="14" t="s">
-        <v>1291</v>
+        <v>1293</v>
       </c>
       <c r="C367" s="14" t="s">
-        <v>1292</v>
+        <v>1294</v>
       </c>
       <c r="D367" s="14" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37383,139 +37496,139 @@
         <v>28</v>
       </c>
       <c r="B368" s="14" t="s">
-        <v>1294</v>
+        <v>1296</v>
       </c>
       <c r="C368" s="14" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="D368" s="14" t="s">
-        <v>1296</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="14" t="s">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="B369" s="14" t="s">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="C369" s="14" t="s">
-        <v>1299</v>
+        <v>1301</v>
       </c>
       <c r="D369" s="14" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="14" t="s">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="B370" s="14" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="C370" s="14" t="s">
-        <v>1303</v>
+        <v>1305</v>
       </c>
       <c r="D370" s="14" t="s">
-        <v>1304</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="14" t="s">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="B371" s="14" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
       <c r="C371" s="14" t="s">
-        <v>1307</v>
+        <v>1309</v>
       </c>
       <c r="D371" s="14" t="s">
-        <v>1308</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="14" t="s">
-        <v>1309</v>
+        <v>1311</v>
       </c>
       <c r="B372" s="14" t="s">
-        <v>1310</v>
+        <v>1312</v>
       </c>
       <c r="C372" s="14" t="s">
-        <v>1311</v>
+        <v>1313</v>
       </c>
       <c r="D372" s="14" t="s">
-        <v>1312</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="14" t="s">
-        <v>1313</v>
+        <v>1315</v>
       </c>
       <c r="B373" s="14" t="s">
-        <v>1314</v>
+        <v>1316</v>
       </c>
       <c r="C373" s="14" t="s">
-        <v>1315</v>
+        <v>1317</v>
       </c>
       <c r="D373" s="14" t="s">
-        <v>1316</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="14" t="s">
-        <v>1317</v>
+        <v>1319</v>
       </c>
       <c r="B374" s="14" t="s">
-        <v>1318</v>
+        <v>1320</v>
       </c>
       <c r="C374" s="14" t="s">
-        <v>1319</v>
+        <v>1321</v>
       </c>
       <c r="D374" s="14" t="s">
-        <v>1320</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="14" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
       <c r="B375" s="14" t="s">
-        <v>1322</v>
+        <v>1324</v>
       </c>
       <c r="C375" s="14" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
       <c r="D375" s="14" t="s">
-        <v>1324</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="14" t="s">
-        <v>1325</v>
+        <v>1327</v>
       </c>
       <c r="B376" s="14" t="s">
-        <v>1326</v>
+        <v>1328</v>
       </c>
       <c r="C376" s="16" t="s">
-        <v>1327</v>
+        <v>1329</v>
       </c>
       <c r="D376" s="16" t="s">
-        <v>1328</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="14" t="s">
-        <v>1329</v>
+        <v>1331</v>
       </c>
       <c r="B377" s="14" t="s">
-        <v>1330</v>
+        <v>1332</v>
       </c>
       <c r="C377" s="16" t="s">
-        <v>1331</v>
+        <v>1333</v>
       </c>
       <c r="D377" s="16" t="s">
-        <v>1332</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37523,13 +37636,13 @@
         <v>27</v>
       </c>
       <c r="B379" s="14" t="s">
-        <v>1333</v>
+        <v>1335</v>
       </c>
       <c r="C379" s="16" t="s">
-        <v>1334</v>
+        <v>1336</v>
       </c>
       <c r="D379" s="16" t="s">
-        <v>1335</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="32.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37537,13 +37650,13 @@
         <v>31</v>
       </c>
       <c r="B380" s="14" t="s">
-        <v>1336</v>
+        <v>1338</v>
       </c>
       <c r="C380" s="16" t="s">
-        <v>1337</v>
+        <v>1339</v>
       </c>
       <c r="D380" s="16" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37551,13 +37664,13 @@
         <v>35</v>
       </c>
       <c r="B381" s="14" t="s">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="C381" s="14" t="s">
-        <v>1340</v>
+        <v>1342</v>
       </c>
       <c r="D381" s="14" t="s">
-        <v>1341</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37565,13 +37678,13 @@
         <v>47</v>
       </c>
       <c r="B382" s="14" t="s">
-        <v>1342</v>
+        <v>1344</v>
       </c>
       <c r="C382" s="14" t="s">
-        <v>1343</v>
+        <v>1345</v>
       </c>
       <c r="D382" s="14" t="s">
-        <v>1344</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37579,123 +37692,153 @@
         <v>53</v>
       </c>
       <c r="B383" s="14" t="s">
-        <v>1345</v>
+        <v>1347</v>
       </c>
       <c r="C383" s="14" t="s">
-        <v>1346</v>
+        <v>1348</v>
       </c>
       <c r="D383" s="14" t="s">
-        <v>1347</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="14" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="B384" s="14" t="s">
-        <v>1349</v>
+        <v>1351</v>
       </c>
       <c r="C384" s="14" t="s">
-        <v>1350</v>
+        <v>1352</v>
       </c>
       <c r="D384" s="14" t="s">
-        <v>1351</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="14" t="s">
-        <v>1352</v>
+        <v>1354</v>
       </c>
       <c r="B385" s="14" t="s">
-        <v>1353</v>
+        <v>1355</v>
       </c>
       <c r="C385" s="16" t="s">
-        <v>1354</v>
+        <v>1356</v>
       </c>
       <c r="D385" s="16" t="s">
-        <v>1355</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="14" t="s">
-        <v>1356</v>
+        <v>1358</v>
       </c>
       <c r="B386" s="14" t="s">
-        <v>1357</v>
+        <v>1359</v>
       </c>
       <c r="C386" s="16" t="s">
-        <v>1358</v>
+        <v>1360</v>
       </c>
       <c r="D386" s="16" t="s">
-        <v>1359</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="14" t="s">
-        <v>1360</v>
+        <v>1362</v>
       </c>
       <c r="B387" s="14" t="s">
-        <v>1361</v>
+        <v>1363</v>
       </c>
       <c r="C387" s="16" t="s">
-        <v>1362</v>
+        <v>1364</v>
       </c>
       <c r="D387" s="16" t="s">
-        <v>1363</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="14" t="s">
-        <v>1364</v>
+        <v>1366</v>
       </c>
       <c r="B388" s="14" t="s">
-        <v>1365</v>
+        <v>1367</v>
       </c>
       <c r="C388" s="14" t="s">
-        <v>1366</v>
+        <v>1368</v>
       </c>
       <c r="D388" s="14" t="s">
-        <v>1367</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="14" t="s">
-        <v>1368</v>
+        <v>1370</v>
       </c>
       <c r="B389" s="14" t="s">
-        <v>1369</v>
+        <v>1371</v>
+      </c>
+      <c r="C389" s="14" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D389" s="14" t="s">
+        <v>1373</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="14" t="s">
-        <v>1370</v>
+        <v>1374</v>
       </c>
       <c r="B390" s="14" t="s">
-        <v>1371</v>
+        <v>1375</v>
+      </c>
+      <c r="C390" s="14" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D390" s="14" t="s">
+        <v>1377</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="14" t="s">
-        <v>1372</v>
+        <v>1378</v>
       </c>
       <c r="B391" s="14" t="s">
-        <v>1373</v>
+        <v>1379</v>
+      </c>
+      <c r="C391" s="14" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D391" s="14" t="s">
+        <v>1381</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="14" t="s">
-        <v>1374</v>
+        <v>1382</v>
       </c>
       <c r="B392" s="14" t="s">
-        <v>1375</v>
+        <v>1383</v>
+      </c>
+      <c r="C392" s="14" t="s">
+        <v>1384</v>
+      </c>
+      <c r="D392" s="14" t="s">
+        <v>1385</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="14" t="s">
-        <v>1376</v>
+        <v>1386</v>
       </c>
       <c r="B393" s="14" t="s">
-        <v>1377</v>
+        <v>1387</v>
+      </c>
+      <c r="C393" s="14" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D393" s="14" t="s">
+        <v>1389</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37703,13 +37846,13 @@
         <v>25</v>
       </c>
       <c r="B395" s="14" t="s">
-        <v>1378</v>
+        <v>1390</v>
       </c>
       <c r="C395" s="14" t="s">
-        <v>1379</v>
+        <v>1391</v>
       </c>
       <c r="D395" s="14" t="s">
-        <v>1380</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37717,13 +37860,13 @@
         <v>29</v>
       </c>
       <c r="B396" s="14" t="s">
-        <v>1381</v>
+        <v>1393</v>
       </c>
       <c r="C396" s="14" t="s">
-        <v>1382</v>
+        <v>1394</v>
       </c>
       <c r="D396" s="14" t="s">
-        <v>1383</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37731,13 +37874,13 @@
         <v>33</v>
       </c>
       <c r="B397" s="14" t="s">
-        <v>1384</v>
+        <v>1396</v>
       </c>
       <c r="C397" s="14" t="s">
-        <v>1385</v>
+        <v>1397</v>
       </c>
       <c r="D397" s="14" t="s">
-        <v>1386</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37745,13 +37888,13 @@
         <v>62</v>
       </c>
       <c r="B398" s="14" t="s">
-        <v>1387</v>
+        <v>1399</v>
       </c>
       <c r="C398" s="14" t="s">
-        <v>1388</v>
+        <v>1400</v>
       </c>
       <c r="D398" s="14" t="s">
-        <v>1389</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37759,13 +37902,13 @@
         <v>69</v>
       </c>
       <c r="B399" s="14" t="s">
-        <v>1390</v>
+        <v>1402</v>
       </c>
       <c r="C399" s="14" t="s">
-        <v>1391</v>
+        <v>1403</v>
       </c>
       <c r="D399" s="14" t="s">
-        <v>1392</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37773,13 +37916,13 @@
         <v>71</v>
       </c>
       <c r="B400" s="14" t="s">
-        <v>1393</v>
+        <v>1405</v>
       </c>
       <c r="C400" s="14" t="s">
-        <v>1394</v>
+        <v>1406</v>
       </c>
       <c r="D400" s="14" t="s">
-        <v>1395</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37787,1393 +37930,1399 @@
         <v>72</v>
       </c>
       <c r="B401" s="14" t="s">
-        <v>1396</v>
+        <v>1408</v>
       </c>
       <c r="C401" s="14" t="s">
-        <v>1397</v>
+        <v>1409</v>
       </c>
       <c r="D401" s="14" t="s">
-        <v>1398</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="14" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="B402" s="14" t="s">
-        <v>1400</v>
+        <v>1412</v>
       </c>
       <c r="C402" s="14" t="s">
-        <v>1401</v>
+        <v>1413</v>
       </c>
       <c r="D402" s="14" t="s">
-        <v>1402</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="14" t="s">
-        <v>1403</v>
+        <v>1415</v>
       </c>
       <c r="B403" s="14" t="s">
-        <v>1404</v>
+        <v>1416</v>
       </c>
       <c r="C403" s="14" t="s">
-        <v>1405</v>
+        <v>1417</v>
       </c>
       <c r="D403" s="14" t="s">
-        <v>1406</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="14" t="s">
-        <v>1407</v>
+        <v>1419</v>
       </c>
       <c r="B404" s="14" t="s">
-        <v>1408</v>
+        <v>1420</v>
       </c>
       <c r="C404" s="14" t="s">
-        <v>1409</v>
+        <v>1421</v>
       </c>
       <c r="D404" s="14" t="s">
-        <v>1410</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="14" t="s">
-        <v>1411</v>
+        <v>1423</v>
       </c>
       <c r="B405" s="14" t="s">
-        <v>1412</v>
+        <v>1424</v>
       </c>
       <c r="C405" s="14" t="s">
-        <v>1413</v>
+        <v>1425</v>
       </c>
       <c r="D405" s="14" t="s">
-        <v>1414</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="14" t="s">
-        <v>1415</v>
+        <v>1427</v>
       </c>
       <c r="B406" s="14" t="s">
-        <v>1416</v>
+        <v>1428</v>
       </c>
       <c r="C406" s="14" t="s">
-        <v>1417</v>
+        <v>1429</v>
       </c>
       <c r="D406" s="14" t="s">
-        <v>1418</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="14" t="s">
-        <v>1419</v>
+        <v>1431</v>
       </c>
       <c r="B407" s="14" t="s">
-        <v>1420</v>
+        <v>1432</v>
       </c>
       <c r="C407" s="14" t="s">
-        <v>1421</v>
+        <v>1433</v>
       </c>
       <c r="D407" s="14" t="s">
-        <v>1422</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="14" t="s">
-        <v>1423</v>
+        <v>1435</v>
       </c>
       <c r="B408" s="14" t="s">
-        <v>1424</v>
+        <v>1436</v>
       </c>
       <c r="C408" s="14" t="s">
-        <v>1425</v>
+        <v>1437</v>
       </c>
       <c r="D408" s="14" t="s">
-        <v>1426</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="14" t="s">
-        <v>1427</v>
+        <v>1439</v>
       </c>
       <c r="B409" s="14" t="s">
-        <v>1428</v>
+        <v>1440</v>
       </c>
       <c r="C409" s="14" t="s">
-        <v>1429</v>
+        <v>1441</v>
       </c>
       <c r="D409" s="14" t="s">
-        <v>1430</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="14" t="s">
-        <v>1431</v>
+        <v>1443</v>
       </c>
       <c r="B410" s="14" t="s">
-        <v>1432</v>
+        <v>1444</v>
       </c>
       <c r="C410" s="14" t="s">
-        <v>1433</v>
+        <v>1445</v>
       </c>
       <c r="D410" s="14" t="s">
-        <v>1434</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="14" t="s">
-        <v>1435</v>
+        <v>1447</v>
       </c>
       <c r="B411" s="14" t="s">
-        <v>1436</v>
+        <v>1448</v>
       </c>
       <c r="C411" s="14" t="s">
-        <v>1437</v>
+        <v>1449</v>
       </c>
       <c r="D411" s="14" t="s">
-        <v>1438</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="14" t="s">
-        <v>1439</v>
+        <v>1451</v>
       </c>
       <c r="B412" s="14" t="s">
-        <v>1440</v>
+        <v>1452</v>
       </c>
       <c r="C412" s="14" t="s">
-        <v>1441</v>
+        <v>1453</v>
       </c>
       <c r="D412" s="14" t="s">
-        <v>1442</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="14" t="s">
-        <v>1443</v>
+        <v>1455</v>
       </c>
       <c r="B413" s="14" t="s">
-        <v>1444</v>
+        <v>1456</v>
       </c>
       <c r="C413" s="14" t="s">
-        <v>1445</v>
+        <v>1457</v>
       </c>
       <c r="D413" s="14" t="s">
-        <v>1446</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="14" t="s">
-        <v>1447</v>
+        <v>1459</v>
       </c>
       <c r="B414" s="14" t="s">
-        <v>1448</v>
+        <v>1460</v>
       </c>
       <c r="C414" s="14" t="s">
-        <v>1449</v>
+        <v>1461</v>
       </c>
       <c r="D414" s="14" t="s">
-        <v>1450</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="14" t="s">
-        <v>1451</v>
+        <v>1463</v>
       </c>
       <c r="B415" s="14" t="s">
-        <v>1396</v>
+        <v>1408</v>
       </c>
       <c r="C415" s="14" t="s">
-        <v>1452</v>
+        <v>1464</v>
       </c>
       <c r="D415" s="14" t="s">
-        <v>1453</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="14" t="s">
-        <v>1454</v>
+        <v>1466</v>
       </c>
       <c r="B416" s="14" t="s">
-        <v>1455</v>
+        <v>1467</v>
       </c>
       <c r="C416" s="14" t="s">
-        <v>1455</v>
+        <v>1467</v>
       </c>
       <c r="D416" s="14" t="s">
-        <v>1455</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="14" t="s">
-        <v>1456</v>
+        <v>1468</v>
       </c>
       <c r="B417" s="14" t="s">
-        <v>1457</v>
+        <v>1469</v>
       </c>
       <c r="C417" s="14" t="s">
-        <v>1458</v>
+        <v>1470</v>
       </c>
       <c r="D417" s="14" t="s">
-        <v>1459</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="14" t="s">
-        <v>1460</v>
+        <v>1472</v>
       </c>
       <c r="B418" s="14" t="s">
-        <v>1461</v>
+        <v>1473</v>
       </c>
       <c r="C418" s="14" t="s">
-        <v>1462</v>
+        <v>1474</v>
       </c>
       <c r="D418" s="14" t="s">
-        <v>1463</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="14" t="s">
-        <v>1464</v>
+        <v>1476</v>
       </c>
       <c r="B419" s="14" t="s">
-        <v>1465</v>
+        <v>1477</v>
       </c>
       <c r="C419" s="14" t="s">
-        <v>1466</v>
+        <v>1478</v>
       </c>
       <c r="D419" s="14" t="s">
-        <v>1467</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="14" t="s">
-        <v>1468</v>
+        <v>1480</v>
       </c>
       <c r="B420" s="14" t="s">
-        <v>1469</v>
+        <v>1481</v>
       </c>
       <c r="C420" s="14" t="s">
-        <v>1470</v>
+        <v>1482</v>
       </c>
       <c r="D420" s="14" t="s">
-        <v>1471</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="14" t="s">
-        <v>1472</v>
+        <v>1484</v>
       </c>
       <c r="B421" s="14" t="s">
-        <v>1473</v>
+        <v>1485</v>
       </c>
       <c r="C421" s="14" t="s">
-        <v>1474</v>
+        <v>1486</v>
       </c>
       <c r="D421" s="14" t="s">
-        <v>1475</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="14" t="s">
-        <v>1476</v>
+        <v>1488</v>
       </c>
       <c r="B422" s="14" t="s">
-        <v>1477</v>
+        <v>1489</v>
       </c>
       <c r="C422" s="14" t="s">
-        <v>1478</v>
+        <v>1490</v>
       </c>
       <c r="D422" s="14" t="s">
-        <v>1479</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="14" t="s">
-        <v>1480</v>
+        <v>1492</v>
       </c>
       <c r="B423" s="14" t="s">
-        <v>1396</v>
+        <v>1408</v>
       </c>
       <c r="C423" s="14" t="s">
-        <v>1452</v>
+        <v>1464</v>
       </c>
       <c r="D423" s="14" t="s">
-        <v>1453</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="14" t="s">
-        <v>1481</v>
+        <v>1493</v>
       </c>
       <c r="B424" s="14" t="s">
-        <v>1482</v>
+        <v>1494</v>
       </c>
       <c r="C424" s="14" t="s">
-        <v>1483</v>
+        <v>1495</v>
       </c>
       <c r="D424" s="14" t="s">
-        <v>1484</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="14" t="s">
-        <v>1485</v>
+        <v>1497</v>
       </c>
       <c r="B425" s="14" t="s">
-        <v>1486</v>
+        <v>1498</v>
       </c>
       <c r="C425" s="14" t="s">
-        <v>1487</v>
+        <v>1499</v>
       </c>
       <c r="D425" s="14" t="s">
-        <v>1488</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="14" t="s">
-        <v>1489</v>
+        <v>1501</v>
       </c>
       <c r="B426" s="14" t="s">
-        <v>1490</v>
+        <v>1502</v>
       </c>
       <c r="C426" s="14" t="s">
-        <v>1491</v>
+        <v>1503</v>
       </c>
       <c r="D426" s="14" t="s">
-        <v>1492</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="14" t="s">
-        <v>1493</v>
+        <v>1505</v>
       </c>
       <c r="B427" s="14" t="s">
-        <v>1494</v>
+        <v>1506</v>
       </c>
       <c r="C427" s="14" t="s">
-        <v>1495</v>
+        <v>1507</v>
       </c>
       <c r="D427" s="14" t="s">
-        <v>1496</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="14" t="s">
-        <v>1497</v>
+        <v>1509</v>
       </c>
       <c r="B428" s="14" t="s">
-        <v>1498</v>
+        <v>1510</v>
       </c>
       <c r="C428" s="14" t="s">
-        <v>1499</v>
+        <v>1511</v>
       </c>
       <c r="D428" s="14" t="s">
-        <v>1500</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="14" t="s">
-        <v>1501</v>
+        <v>1513</v>
       </c>
       <c r="B429" s="14" t="s">
-        <v>1502</v>
+        <v>1514</v>
       </c>
       <c r="C429" s="14" t="s">
-        <v>1503</v>
+        <v>1515</v>
       </c>
       <c r="D429" s="14" t="s">
-        <v>1504</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="14" t="s">
-        <v>1505</v>
+        <v>1517</v>
       </c>
       <c r="B430" s="14" t="s">
-        <v>1506</v>
+        <v>1518</v>
       </c>
       <c r="C430" s="14" t="s">
-        <v>1507</v>
+        <v>1519</v>
       </c>
       <c r="D430" s="14" t="s">
-        <v>1508</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="14" t="s">
-        <v>1509</v>
+        <v>1521</v>
       </c>
       <c r="B431" s="14" t="s">
-        <v>1510</v>
+        <v>1522</v>
       </c>
       <c r="C431" s="14" t="s">
-        <v>1511</v>
+        <v>1523</v>
       </c>
       <c r="D431" s="14" t="s">
-        <v>1512</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="14" t="s">
-        <v>1513</v>
+        <v>1525</v>
       </c>
       <c r="B432" s="14" t="s">
-        <v>1514</v>
+        <v>1526</v>
       </c>
       <c r="C432" s="14" t="s">
-        <v>1515</v>
+        <v>1527</v>
       </c>
       <c r="D432" s="14" t="s">
-        <v>1516</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="14" t="s">
-        <v>1517</v>
+        <v>1529</v>
       </c>
       <c r="B433" s="14" t="s">
-        <v>1518</v>
+        <v>1530</v>
       </c>
       <c r="C433" s="14" t="s">
-        <v>1519</v>
+        <v>1531</v>
       </c>
       <c r="D433" s="14" t="s">
-        <v>1520</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="14" t="s">
-        <v>1521</v>
+        <v>1533</v>
       </c>
       <c r="B434" s="14" t="s">
-        <v>1522</v>
+        <v>1534</v>
       </c>
       <c r="C434" s="14" t="s">
-        <v>1523</v>
+        <v>1535</v>
       </c>
       <c r="D434" s="14" t="s">
-        <v>1524</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="14" t="s">
-        <v>1525</v>
+        <v>1537</v>
       </c>
       <c r="B435" s="14" t="s">
-        <v>1526</v>
+        <v>1538</v>
       </c>
       <c r="C435" s="14" t="s">
-        <v>1527</v>
+        <v>1539</v>
       </c>
       <c r="D435" s="14" t="s">
-        <v>1528</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="14" t="s">
-        <v>1529</v>
+        <v>1541</v>
       </c>
       <c r="B436" s="14" t="s">
-        <v>1530</v>
+        <v>1542</v>
       </c>
       <c r="C436" s="14" t="s">
-        <v>1531</v>
+        <v>1543</v>
       </c>
       <c r="D436" s="14" t="s">
-        <v>1532</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="14" t="s">
-        <v>1533</v>
+        <v>1545</v>
       </c>
       <c r="B438" s="14" t="s">
-        <v>1534</v>
+        <v>1546</v>
       </c>
       <c r="C438" s="14" t="s">
-        <v>1535</v>
+        <v>1547</v>
       </c>
       <c r="D438" s="14" t="s">
-        <v>1536</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="14" t="s">
-        <v>1537</v>
+        <v>1549</v>
       </c>
       <c r="B439" s="14" t="s">
-        <v>1538</v>
+        <v>1550</v>
       </c>
       <c r="C439" s="14" t="s">
-        <v>1539</v>
+        <v>1551</v>
       </c>
       <c r="D439" s="14" t="s">
-        <v>1540</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="14" t="s">
-        <v>1541</v>
+        <v>1553</v>
       </c>
       <c r="B440" s="14" t="s">
-        <v>1542</v>
+        <v>1554</v>
       </c>
       <c r="C440" s="14" t="s">
-        <v>1543</v>
+        <v>1555</v>
       </c>
       <c r="D440" s="14" t="s">
-        <v>1544</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="14" t="s">
-        <v>1545</v>
+        <v>1557</v>
       </c>
       <c r="B441" s="14" t="s">
-        <v>1546</v>
+        <v>1558</v>
       </c>
       <c r="C441" s="14" t="s">
-        <v>1547</v>
+        <v>1559</v>
       </c>
       <c r="D441" s="14" t="s">
-        <v>1548</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="14" t="s">
-        <v>1549</v>
+        <v>1561</v>
       </c>
       <c r="B442" s="14" t="s">
-        <v>1550</v>
+        <v>1562</v>
       </c>
       <c r="C442" s="14" t="s">
-        <v>1551</v>
+        <v>1563</v>
       </c>
       <c r="D442" s="14" t="s">
-        <v>1552</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="14" t="s">
-        <v>1553</v>
+        <v>1565</v>
       </c>
       <c r="B443" s="14" t="s">
-        <v>1554</v>
+        <v>1566</v>
       </c>
       <c r="C443" s="14" t="s">
-        <v>1555</v>
+        <v>1567</v>
       </c>
       <c r="D443" s="14" t="s">
-        <v>1556</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="14" t="s">
-        <v>1557</v>
+        <v>1569</v>
       </c>
       <c r="B444" s="14" t="s">
-        <v>1558</v>
+        <v>1570</v>
       </c>
       <c r="C444" s="14" t="s">
-        <v>1559</v>
+        <v>1571</v>
       </c>
       <c r="D444" s="14" t="s">
-        <v>1560</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="14" t="s">
-        <v>1561</v>
+        <v>1573</v>
       </c>
       <c r="B445" s="14" t="s">
-        <v>1562</v>
+        <v>1574</v>
       </c>
       <c r="C445" s="14" t="s">
-        <v>1563</v>
+        <v>1575</v>
       </c>
       <c r="D445" s="14" t="s">
-        <v>1564</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="14" t="s">
-        <v>1565</v>
+        <v>1577</v>
       </c>
       <c r="B446" s="14" t="s">
-        <v>1566</v>
+        <v>1578</v>
       </c>
       <c r="C446" s="14" t="s">
-        <v>1567</v>
+        <v>1579</v>
       </c>
       <c r="D446" s="14" t="s">
-        <v>1568</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="14" t="s">
-        <v>1569</v>
+        <v>1581</v>
       </c>
       <c r="B447" s="14" t="s">
-        <v>1570</v>
+        <v>1582</v>
       </c>
       <c r="C447" s="14" t="s">
-        <v>1571</v>
+        <v>1583</v>
       </c>
       <c r="D447" s="14" t="s">
-        <v>1572</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="14" t="s">
-        <v>1573</v>
+        <v>1585</v>
       </c>
       <c r="B448" s="14" t="s">
-        <v>1574</v>
+        <v>1586</v>
       </c>
       <c r="C448" s="14" t="s">
-        <v>1575</v>
+        <v>1587</v>
       </c>
       <c r="D448" s="14" t="s">
-        <v>1576</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="14" t="s">
-        <v>1577</v>
+        <v>1589</v>
       </c>
       <c r="B449" s="14" t="s">
-        <v>1578</v>
+        <v>1590</v>
       </c>
       <c r="C449" s="14" t="s">
-        <v>1579</v>
+        <v>1591</v>
       </c>
       <c r="D449" s="14" t="s">
-        <v>1580</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="14" t="s">
-        <v>1581</v>
+        <v>1593</v>
       </c>
       <c r="B450" s="14" t="s">
-        <v>1582</v>
+        <v>1594</v>
       </c>
       <c r="C450" s="14" t="s">
-        <v>1583</v>
+        <v>1595</v>
       </c>
       <c r="D450" s="14" t="s">
-        <v>1584</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="14" t="s">
-        <v>1585</v>
+        <v>1597</v>
       </c>
       <c r="B451" s="14" t="s">
-        <v>1586</v>
+        <v>1598</v>
       </c>
       <c r="C451" s="14" t="s">
-        <v>1587</v>
+        <v>1599</v>
       </c>
       <c r="D451" s="14" t="s">
-        <v>1588</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="14" t="s">
-        <v>1589</v>
+        <v>1601</v>
       </c>
       <c r="B452" s="14" t="s">
-        <v>1590</v>
+        <v>1602</v>
       </c>
       <c r="C452" s="14" t="s">
-        <v>1591</v>
+        <v>1603</v>
       </c>
       <c r="D452" s="14" t="s">
-        <v>1592</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="14" t="s">
-        <v>1593</v>
+        <v>1605</v>
       </c>
       <c r="B453" s="14" t="s">
-        <v>1594</v>
+        <v>1606</v>
       </c>
       <c r="C453" s="14" t="s">
-        <v>1595</v>
+        <v>1607</v>
       </c>
       <c r="D453" s="14" t="s">
-        <v>1596</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="14" t="s">
-        <v>1597</v>
+        <v>1609</v>
       </c>
       <c r="B454" s="14" t="s">
-        <v>1598</v>
+        <v>1610</v>
       </c>
       <c r="C454" s="14" t="s">
-        <v>1599</v>
+        <v>1611</v>
       </c>
       <c r="D454" s="14" t="s">
-        <v>1600</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="14" t="s">
-        <v>1601</v>
+        <v>1613</v>
       </c>
       <c r="B455" s="14" t="s">
-        <v>1602</v>
+        <v>1614</v>
       </c>
       <c r="C455" s="14" t="s">
-        <v>1603</v>
+        <v>1615</v>
       </c>
       <c r="D455" s="14" t="s">
-        <v>1604</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="14" t="s">
-        <v>1605</v>
+        <v>1617</v>
       </c>
       <c r="B456" s="14" t="s">
-        <v>1606</v>
+        <v>1618</v>
       </c>
       <c r="C456" s="14" t="s">
-        <v>1607</v>
+        <v>1619</v>
       </c>
       <c r="D456" s="14" t="s">
-        <v>1608</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="14" t="s">
-        <v>1609</v>
+        <v>1621</v>
       </c>
       <c r="B457" s="14" t="s">
-        <v>1610</v>
+        <v>1622</v>
       </c>
       <c r="C457" s="14" t="s">
-        <v>1611</v>
+        <v>1623</v>
       </c>
       <c r="D457" s="14" t="s">
-        <v>1612</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="14" t="s">
-        <v>1613</v>
+        <v>1625</v>
       </c>
       <c r="B458" s="14" t="s">
-        <v>1614</v>
+        <v>1626</v>
       </c>
       <c r="C458" s="14" t="s">
-        <v>1615</v>
+        <v>1627</v>
       </c>
       <c r="D458" s="14" t="s">
-        <v>1616</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="14" t="s">
-        <v>1617</v>
+        <v>1629</v>
       </c>
       <c r="B459" s="14" t="s">
-        <v>1618</v>
+        <v>1630</v>
       </c>
       <c r="C459" s="14" t="s">
-        <v>1619</v>
+        <v>1631</v>
       </c>
       <c r="D459" s="14" t="s">
-        <v>1620</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="14" t="s">
-        <v>1621</v>
+        <v>1633</v>
       </c>
       <c r="B460" s="14" t="s">
-        <v>1622</v>
+        <v>1634</v>
       </c>
       <c r="C460" s="14" t="s">
-        <v>1623</v>
+        <v>1635</v>
       </c>
       <c r="D460" s="14" t="s">
-        <v>1624</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="14" t="s">
-        <v>1625</v>
+        <v>1637</v>
       </c>
       <c r="B461" s="14" t="s">
-        <v>1626</v>
+        <v>1638</v>
       </c>
       <c r="C461" s="14" t="s">
-        <v>1627</v>
+        <v>1639</v>
       </c>
       <c r="D461" s="14" t="s">
-        <v>1628</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="14" t="s">
-        <v>1629</v>
+        <v>1641</v>
       </c>
       <c r="B462" s="14" t="s">
-        <v>1630</v>
+        <v>1642</v>
       </c>
       <c r="C462" s="14" t="s">
-        <v>1631</v>
+        <v>1643</v>
       </c>
       <c r="D462" s="14" t="s">
-        <v>1632</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="14" t="s">
-        <v>1633</v>
+        <v>1645</v>
       </c>
       <c r="B463" s="14" t="s">
-        <v>1634</v>
+        <v>1646</v>
       </c>
       <c r="C463" s="14" t="s">
-        <v>1635</v>
+        <v>1647</v>
       </c>
       <c r="D463" s="14" t="s">
-        <v>1636</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="14" t="s">
-        <v>1637</v>
+        <v>1649</v>
       </c>
       <c r="B464" s="14" t="s">
-        <v>1638</v>
+        <v>1650</v>
       </c>
       <c r="C464" s="14" t="s">
-        <v>1639</v>
+        <v>1651</v>
       </c>
       <c r="D464" s="14" t="s">
-        <v>1640</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="14" t="s">
-        <v>1641</v>
+        <v>1653</v>
       </c>
       <c r="B465" s="14" t="s">
-        <v>1642</v>
+        <v>1654</v>
       </c>
       <c r="C465" s="14" t="s">
-        <v>1643</v>
+        <v>1655</v>
       </c>
       <c r="D465" s="14" t="s">
-        <v>1644</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="14" t="s">
-        <v>1645</v>
+        <v>1657</v>
       </c>
       <c r="B466" s="14" t="s">
-        <v>1646</v>
+        <v>1658</v>
       </c>
       <c r="C466" s="14" t="s">
-        <v>1647</v>
+        <v>1659</v>
       </c>
       <c r="D466" s="14" t="s">
-        <v>1648</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="14" t="s">
-        <v>1649</v>
+        <v>1661</v>
       </c>
       <c r="B467" s="14" t="s">
-        <v>1650</v>
+        <v>1662</v>
       </c>
       <c r="C467" s="14" t="s">
-        <v>1651</v>
+        <v>1663</v>
       </c>
       <c r="D467" s="14" t="s">
-        <v>1652</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="14" t="s">
-        <v>1653</v>
+        <v>1665</v>
       </c>
       <c r="B468" s="14" t="s">
-        <v>1654</v>
+        <v>1666</v>
       </c>
       <c r="C468" s="14" t="s">
-        <v>1655</v>
+        <v>1667</v>
       </c>
       <c r="D468" s="14" t="s">
-        <v>1656</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="14" t="s">
-        <v>1657</v>
+        <v>1669</v>
       </c>
       <c r="B469" s="14" t="s">
-        <v>1658</v>
+        <v>1670</v>
       </c>
       <c r="C469" s="14" t="s">
-        <v>1659</v>
+        <v>1671</v>
       </c>
       <c r="D469" s="14" t="s">
-        <v>1660</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="14" t="s">
-        <v>1661</v>
+        <v>1673</v>
       </c>
       <c r="B470" s="14" t="s">
-        <v>1662</v>
+        <v>1674</v>
       </c>
       <c r="C470" s="14" t="s">
-        <v>1663</v>
+        <v>1675</v>
       </c>
       <c r="D470" s="14" t="s">
-        <v>1664</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="14" t="s">
-        <v>1665</v>
+        <v>1677</v>
       </c>
       <c r="B471" s="14" t="s">
-        <v>1666</v>
+        <v>1678</v>
       </c>
       <c r="C471" s="14" t="s">
-        <v>1667</v>
+        <v>1679</v>
       </c>
       <c r="D471" s="14" t="s">
-        <v>1668</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="14" t="s">
-        <v>1669</v>
+        <v>1681</v>
       </c>
       <c r="B472" s="14" t="s">
-        <v>1670</v>
+        <v>1682</v>
       </c>
       <c r="C472" s="14" t="s">
-        <v>1671</v>
+        <v>1683</v>
       </c>
       <c r="D472" s="14" t="s">
-        <v>1672</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="14" t="s">
-        <v>1673</v>
+        <v>1685</v>
       </c>
       <c r="B473" s="14" t="s">
-        <v>1674</v>
+        <v>1686</v>
       </c>
       <c r="C473" s="14" t="s">
-        <v>1675</v>
+        <v>1687</v>
       </c>
       <c r="D473" s="14" t="s">
-        <v>1676</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="14" t="s">
-        <v>1677</v>
+        <v>1689</v>
       </c>
       <c r="B474" s="14" t="s">
-        <v>1678</v>
+        <v>1690</v>
       </c>
       <c r="C474" s="14" t="s">
-        <v>1679</v>
+        <v>1691</v>
       </c>
       <c r="D474" s="14" t="s">
-        <v>1680</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="14" t="s">
-        <v>1681</v>
+        <v>1693</v>
       </c>
       <c r="B475" s="14" t="s">
-        <v>1682</v>
+        <v>1694</v>
       </c>
       <c r="C475" s="14" t="s">
-        <v>1683</v>
+        <v>1695</v>
       </c>
       <c r="D475" s="14" t="s">
-        <v>1684</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="14" t="s">
-        <v>1685</v>
+        <v>1697</v>
       </c>
       <c r="B476" s="14" t="s">
-        <v>1686</v>
+        <v>1698</v>
       </c>
       <c r="C476" s="14" t="s">
-        <v>1687</v>
+        <v>1699</v>
       </c>
       <c r="D476" s="14" t="s">
-        <v>1688</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="14" t="s">
-        <v>1689</v>
+        <v>1701</v>
       </c>
       <c r="B477" s="14" t="s">
-        <v>1690</v>
+        <v>1702</v>
       </c>
       <c r="C477" s="14" t="s">
-        <v>1691</v>
+        <v>1703</v>
       </c>
       <c r="D477" s="14" t="s">
-        <v>1692</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="14" t="s">
-        <v>1693</v>
+        <v>1705</v>
       </c>
       <c r="B478" s="14" t="s">
-        <v>1694</v>
+        <v>1706</v>
       </c>
       <c r="C478" s="14" t="s">
-        <v>1695</v>
+        <v>1707</v>
       </c>
       <c r="D478" s="14" t="s">
-        <v>1696</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="14" t="s">
-        <v>1697</v>
+        <v>1709</v>
       </c>
       <c r="B479" s="14" t="s">
-        <v>1698</v>
+        <v>1710</v>
       </c>
       <c r="C479" s="14" t="s">
-        <v>1699</v>
+        <v>1711</v>
       </c>
       <c r="D479" s="14" t="s">
-        <v>1700</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="14" t="s">
-        <v>1701</v>
+        <v>1713</v>
       </c>
       <c r="B480" s="14" t="s">
-        <v>1702</v>
+        <v>1714</v>
       </c>
       <c r="C480" s="14" t="s">
-        <v>1703</v>
+        <v>1715</v>
       </c>
       <c r="D480" s="14" t="s">
-        <v>1704</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="14" t="s">
-        <v>1705</v>
+        <v>1717</v>
       </c>
       <c r="B481" s="14" t="s">
-        <v>1706</v>
+        <v>1718</v>
       </c>
       <c r="C481" s="14" t="s">
-        <v>1707</v>
+        <v>1719</v>
       </c>
       <c r="D481" s="14" t="s">
-        <v>1708</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="14" t="s">
-        <v>1709</v>
+        <v>1721</v>
       </c>
       <c r="B482" s="14" t="s">
-        <v>1710</v>
+        <v>1722</v>
       </c>
       <c r="C482" s="14" t="s">
-        <v>1711</v>
+        <v>1723</v>
       </c>
       <c r="D482" s="14" t="s">
-        <v>1712</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="14" t="s">
-        <v>1713</v>
+        <v>1725</v>
       </c>
       <c r="B483" s="14" t="s">
-        <v>1714</v>
+        <v>1726</v>
       </c>
       <c r="C483" s="14" t="s">
-        <v>1715</v>
+        <v>1727</v>
       </c>
       <c r="D483" s="14" t="s">
-        <v>1716</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="14" t="s">
-        <v>1717</v>
+        <v>1729</v>
       </c>
       <c r="B484" s="14" t="s">
-        <v>1718</v>
+        <v>1730</v>
       </c>
       <c r="C484" s="14" t="s">
-        <v>1719</v>
+        <v>1731</v>
       </c>
       <c r="D484" s="14" t="s">
-        <v>1720</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="14" t="s">
-        <v>1721</v>
+        <v>1733</v>
       </c>
       <c r="B486" s="14" t="s">
-        <v>1722</v>
+        <v>1734</v>
       </c>
       <c r="C486" s="16" t="s">
-        <v>1723</v>
+        <v>1735</v>
       </c>
       <c r="D486" s="16" t="s">
-        <v>1724</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="14" t="s">
-        <v>1725</v>
+        <v>1737</v>
       </c>
       <c r="B487" s="14" t="s">
-        <v>1726</v>
+        <v>1738</v>
       </c>
       <c r="C487" s="16" t="s">
-        <v>1727</v>
+        <v>1739</v>
       </c>
       <c r="D487" s="16" t="s">
-        <v>1728</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="14" t="s">
-        <v>1729</v>
+        <v>1741</v>
       </c>
       <c r="B488" s="14" t="s">
-        <v>1730</v>
+        <v>1742</v>
       </c>
       <c r="C488" s="16" t="s">
-        <v>1731</v>
+        <v>1743</v>
       </c>
       <c r="D488" s="16" t="s">
-        <v>1732</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="14" t="s">
-        <v>1733</v>
+        <v>1745</v>
       </c>
       <c r="B489" s="14" t="s">
-        <v>1734</v>
+        <v>1746</v>
       </c>
       <c r="C489" s="16" t="s">
-        <v>1735</v>
+        <v>1747</v>
       </c>
       <c r="D489" s="16" t="s">
-        <v>1736</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="14" t="s">
-        <v>1737</v>
+        <v>1749</v>
       </c>
       <c r="B490" s="14" t="s">
-        <v>1738</v>
+        <v>1750</v>
       </c>
       <c r="C490" s="16" t="s">
-        <v>1739</v>
+        <v>1751</v>
       </c>
       <c r="D490" s="16" t="s">
-        <v>1740</v>
+        <v>1752</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="14" t="s">
-        <v>1741</v>
+        <v>1753</v>
       </c>
       <c r="B491" s="14" t="s">
-        <v>1742</v>
+        <v>1754</v>
       </c>
       <c r="C491" s="16" t="s">
-        <v>1743</v>
+        <v>1755</v>
       </c>
       <c r="D491" s="16" t="s">
-        <v>1744</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="14" t="s">
-        <v>1745</v>
+        <v>1757</v>
       </c>
       <c r="B492" s="14" t="s">
-        <v>1746</v>
+        <v>1758</v>
       </c>
       <c r="C492" s="16" t="s">
-        <v>1747</v>
+        <v>1759</v>
       </c>
       <c r="D492" s="16" t="s">
-        <v>1748</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="14" t="s">
-        <v>1749</v>
+        <v>1761</v>
       </c>
       <c r="B493" s="14" t="s">
-        <v>1750</v>
+        <v>1762</v>
       </c>
       <c r="C493" s="16" t="s">
-        <v>1751</v>
+        <v>1763</v>
       </c>
       <c r="D493" s="16" t="s">
-        <v>1752</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="33.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="14" t="s">
-        <v>1753</v>
+        <v>1765</v>
       </c>
       <c r="B494" s="14" t="s">
-        <v>1754</v>
+        <v>1766</v>
       </c>
       <c r="C494" s="16" t="s">
-        <v>1755</v>
+        <v>1767</v>
       </c>
       <c r="D494" s="16" t="s">
-        <v>1756</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="16.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A495" s="14" t="s">
-        <v>1757</v>
+        <v>1769</v>
       </c>
       <c r="B495" s="17" t="s">
-        <v>1758</v>
+        <v>1770</v>
       </c>
       <c r="C495" s="16" t="s">
-        <v>1759</v>
+        <v>1771</v>
       </c>
       <c r="D495" s="16" t="s">
-        <v>1760</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="14" t="s">
-        <v>1761</v>
+        <v>1773</v>
       </c>
       <c r="B496" s="14" t="s">
-        <v>1762</v>
+        <v>1774</v>
       </c>
       <c r="C496" s="14" t="s">
-        <v>1763</v>
+        <v>1775</v>
       </c>
       <c r="D496" s="14" t="s">
-        <v>1764</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="14" t="s">
-        <v>1765</v>
+        <v>1777</v>
       </c>
       <c r="B497" s="14" t="s">
-        <v>1766</v>
+        <v>1778</v>
       </c>
       <c r="C497" s="14" t="s">
-        <v>1767</v>
+        <v>1779</v>
       </c>
       <c r="D497" s="14" t="s">
-        <v>1768</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="14" t="s">
-        <v>1769</v>
+        <v>1781</v>
       </c>
       <c r="B498" s="14" t="s">
-        <v>1770</v>
+        <v>1782</v>
       </c>
       <c r="C498" s="16" t="s">
-        <v>1354</v>
+        <v>1356</v>
       </c>
       <c r="D498" s="16" t="s">
-        <v>1355</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="14" t="s">
-        <v>1771</v>
+        <v>1783</v>
       </c>
       <c r="B499" s="14" t="s">
-        <v>1772</v>
+        <v>1784</v>
       </c>
       <c r="C499" s="16" t="s">
-        <v>1358</v>
+        <v>1360</v>
       </c>
       <c r="D499" s="16" t="s">
-        <v>1359</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="22.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="14" t="s">
-        <v>1773</v>
+        <v>1785</v>
       </c>
       <c r="B500" s="14" t="s">
-        <v>1774</v>
+        <v>1786</v>
       </c>
       <c r="C500" s="16" t="s">
-        <v>1362</v>
+        <v>1364</v>
       </c>
       <c r="D500" s="16" t="s">
-        <v>1363</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="18" t="s">
-        <v>1775</v>
+        <v>1787</v>
       </c>
       <c r="B501" s="14" t="s">
-        <v>1776</v>
+        <v>1788</v>
+      </c>
+      <c r="C501" s="14" t="s">
+        <v>1789</v>
+      </c>
+      <c r="D501" s="14" t="s">
+        <v>1790</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="14" t="s">
-        <v>1777</v>
+        <v>1791</v>
       </c>
       <c r="B502" s="14" t="s">
-        <v>1778</v>
+        <v>1792</v>
       </c>
       <c r="C502" s="14" t="s">
-        <v>1779</v>
+        <v>1793</v>
       </c>
       <c r="D502" s="14" t="s">
-        <v>1780</v>
+        <v>1794</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update household member PT translation
April requests row 42
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -4683,7 +4683,7 @@
     <t xml:space="preserve">1. Household member</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Número do agregado familiar</t>
+    <t xml:space="preserve">1. Membro do agregado familiar</t>
   </si>
   <si>
     <t xml:space="preserve">1. Mwanakaya</t>
@@ -5807,9 +5807,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="7.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6858,19 +6858,19 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="40.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="10.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="9.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="10.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8367,13 +8367,13 @@
       <selection pane="bottomLeft" activeCell="C169" activeCellId="0" sqref="C169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13651,17 +13651,17 @@
       <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="8.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31320,17 +31320,17 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="7.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32463,17 +32463,17 @@
   </sheetPr>
   <dimension ref="A1:D491"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A387" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B399" activeCellId="0" sqref="B399"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A417" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D427" activeCellId="0" sqref="D427"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.21484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="33.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="35.54"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="10.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="31.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="33.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="10.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update epilipsy PT translation
April requests row 43
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -3177,7 +3177,7 @@
     <t xml:space="preserve">Treatment for epilepsy</t>
   </si>
   <si>
-    <t xml:space="preserve">Tratamento para a epilepsia</t>
+    <t xml:space="preserve">Tratamento para a epilepsia (convulsões)</t>
   </si>
   <si>
     <t xml:space="preserve">Matibabu ya kifafa</t>
@@ -5807,9 +5807,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="7.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6858,19 +6858,19 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="9.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="9.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="9.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8367,13 +8367,13 @@
       <selection pane="bottomLeft" activeCell="C169" activeCellId="0" sqref="C169"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13651,17 +13651,17 @@
       <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="7.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="7.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31320,17 +31320,17 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.96875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="7.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32464,16 +32464,16 @@
   <dimension ref="A1:D491"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A417" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D427" activeCellId="0" sqref="D427"/>
+      <selection pane="bottomLeft" activeCell="C188" activeCellId="0" sqref="C188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.21484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="31.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="33.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="10.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="29.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="31.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="9.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Change constipation to cold
April requests row 44
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -723,7 +723,7 @@
     <t xml:space="preserve">Malaria</t>
   </si>
   <si>
-    <t xml:space="preserve">Constipation</t>
+    <t xml:space="preserve">Cold</t>
   </si>
   <si>
     <t xml:space="preserve">Fever</t>
@@ -5807,9 +5807,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="7.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="6.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6858,19 +6858,19 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="9.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="8.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8361,19 +8361,19 @@
   </sheetPr>
   <dimension ref="A1:Y1015"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C169" activeCellId="0" sqref="C169"/>
+      <selection pane="bottomLeft" activeCell="B172" activeCellId="0" sqref="B172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13651,17 +13651,17 @@
       <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="7.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="6.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31320,17 +31320,17 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.22265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="7.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="6.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32463,17 +32463,17 @@
   </sheetPr>
   <dimension ref="A1:D491"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C188" activeCellId="0" sqref="C188"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="29.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="31.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="30.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix PT translation of worms
April requests row 45
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -2178,7 +2178,7 @@
     <t xml:space="preserve">Tatizo la afya ya kiakili</t>
   </si>
   <si>
-    <t xml:space="preserve">Parasitas</t>
+    <t xml:space="preserve">Vermes/Lombrigas</t>
   </si>
   <si>
     <t xml:space="preserve">Minyoo</t>
@@ -5043,7 +5043,7 @@
     <t xml:space="preserve">22. Has this participant recently passed worms in the stool in the last 15 days?</t>
   </si>
   <si>
-    <t xml:space="preserve">22. O participante teve parasitas nas fezes nos últimos 15 dias?</t>
+    <t xml:space="preserve">22. O participante teve vermes/lombrigas nas fezes nos últimos 15 dias?</t>
   </si>
   <si>
     <t xml:space="preserve">22. Je, mshiriki huyu alitoa kinyesi chenye minyoo hivi karibuni katika siku 15 zilizopita?</t>
@@ -5807,9 +5807,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="6.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="6.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6858,19 +6858,19 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="8.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="8.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="8.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8361,19 +8361,19 @@
   </sheetPr>
   <dimension ref="A1:Y1015"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B172" activeCellId="0" sqref="B172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13651,17 +13651,17 @@
       <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="6.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="6.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31320,17 +31320,17 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="6.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="6.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32463,17 +32463,17 @@
   </sheetPr>
   <dimension ref="A1:D491"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A447" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
+      <selection pane="bottomLeft" activeCell="B457" activeCellId="0" sqref="B457"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.65625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="28.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="30.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="26.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="28.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="8.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update PT translation of census q18
April requests row 46
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -4995,7 +4995,7 @@
     <t xml:space="preserve">18. Does this participant have any deficiency, lesion or invalidity?</t>
   </si>
   <si>
-    <t xml:space="preserve">18. O participante tem alguma deficiência, lesão ou invalidez?</t>
+    <t xml:space="preserve">18. O participante vive com alguma deficiência, lesão ou invalidez?</t>
   </si>
   <si>
     <t xml:space="preserve">18. Mshiriki huyu ana upungufu wowote, jeraha au ugonjwa?</t>
@@ -5807,9 +5807,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="6.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="6.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6858,19 +6858,19 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="8.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="8.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8367,13 +8367,13 @@
       <selection pane="bottomLeft" activeCell="B172" activeCellId="0" sqref="B172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="8.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="7.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13651,17 +13651,17 @@
       <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="6.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="7.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31320,17 +31320,17 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.84375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="6.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="6.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32466,14 +32466,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A447" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B457" activeCellId="0" sqref="B457"/>
+      <selection pane="bottomLeft" activeCell="C454" activeCellId="0" sqref="C454"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="26.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="28.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="25.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="8.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update PT translation of census q20
April requests row 47
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
+++ b/odkx/app/config/tables/hh_member/forms/hh_member/hh_member.xlsx
@@ -5019,7 +5019,7 @@
     <t xml:space="preserve">20. Does this participant have tunga?</t>
   </si>
   <si>
-    <t xml:space="preserve">20. O participante tem tunga?</t>
+    <t xml:space="preserve">20. O participante tem tunga? (matequenha)</t>
   </si>
   <si>
     <t xml:space="preserve">20. Je, mshiriki huyu ana tunga?</t>
@@ -5807,9 +5807,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="5.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6858,19 +6858,19 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="7.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="8.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="7.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="15" style="0" width="7.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8367,13 +8367,13 @@
       <selection pane="bottomLeft" activeCell="B172" activeCellId="0" sqref="B172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="8.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="7.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="7.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="7.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13651,17 +13651,17 @@
       <selection pane="topLeft" activeCell="D64" activeCellId="0" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="6.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="7.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="9" style="0" width="5.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="7.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31320,17 +31320,17 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="5.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -32466,14 +32466,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A447" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C454" activeCellId="0" sqref="C454"/>
+      <selection pane="bottomLeft" activeCell="C456" activeCellId="0" sqref="C456"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="25.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="27"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="8.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="23.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="6" width="25.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="15" width="7.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>